<commit_message>
added income and population data to new-grocery-store-data (up to row #100 in Excel file)
</commit_message>
<xml_diff>
--- a/moreWorkingData.xlsx
+++ b/moreWorkingData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Navi\Documents\School\CS 438 (Big Data)\LetsGetThisBread\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mitchell.nguyen/school/senior year/spring 2019/big data/zzz letsGetThisBread/github/LetsGetThisBread/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BB7E2E-B45D-49BC-8872-561DB315661F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B165DE6-B9DA-8944-9DAA-0292F410622D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="458" windowWidth="25598" windowHeight="15038" xr2:uid="{224DDC23-A165-FE48-9542-0EB173C9A9C5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{224DDC23-A165-FE48-9542-0EB173C9A9C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1071,7 +1071,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1081,6 +1081,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1107,7 +1114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1115,6 +1122,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1429,24 +1438,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9739F2B-2F3B-DD45-BA29-3AA82495FC82}">
-  <dimension ref="A1:G206"/>
+  <dimension ref="A1:H206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B182" zoomScale="75" workbookViewId="0">
-      <selection activeCell="D206" sqref="D206"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="75" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.8125" customWidth="1"/>
-    <col min="2" max="2" width="12.3125" customWidth="1"/>
-    <col min="3" max="3" width="69.6875" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="69.6640625" customWidth="1"/>
     <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="25.6875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="27.1875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.1640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="22" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1469,7 +1478,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1492,7 +1501,7 @@
         <v>23200</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1515,7 +1524,7 @@
         <v>29007</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1538,7 +1547,7 @@
         <v>22668</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1561,7 +1570,7 @@
         <v>8395</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1584,7 +1593,7 @@
         <v>27612</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1607,7 +1616,7 @@
         <v>30072</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1630,7 +1639,7 @@
         <v>9915</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1653,7 +1662,7 @@
         <v>23200</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1676,7 +1685,7 @@
         <v>30688</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1699,7 +1708,7 @@
         <v>10676</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1722,7 +1731,7 @@
         <v>22668</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1745,7 +1754,7 @@
         <v>37097</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1768,7 +1777,7 @@
         <v>45454</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -1791,7 +1800,7 @@
         <v>37097</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1814,7 +1823,7 @@
         <v>30072</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1837,7 +1846,7 @@
         <v>28254</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1860,7 +1869,7 @@
         <v>17978</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1883,7 +1892,7 @@
         <v>27612</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1906,7 +1915,7 @@
         <v>29007</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -1929,7 +1938,7 @@
         <v>45454</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1952,7 +1961,7 @@
         <v>28254</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1975,7 +1984,7 @@
         <v>27422</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1998,7 +2007,7 @@
         <v>31968</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -2021,7 +2030,7 @@
         <v>30072</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -2044,7 +2053,7 @@
         <v>12340</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -2067,7 +2076,7 @@
         <v>10676</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -2090,7 +2099,7 @@
         <v>27612</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -2113,7 +2122,7 @@
         <v>30072</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -2136,7 +2145,7 @@
         <v>8395</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -2159,7 +2168,7 @@
         <v>10676</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -2182,7 +2191,7 @@
         <v>37062</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -2205,7 +2214,7 @@
         <v>22668</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -2228,7 +2237,7 @@
         <v>29007</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -2251,7 +2260,7 @@
         <v>27422</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -2274,7 +2283,7 @@
         <v>27705</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -2297,7 +2306,7 @@
         <v>17978</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>45</v>
       </c>
@@ -2320,7 +2329,7 @@
         <v>27612</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -2343,7 +2352,7 @@
         <v>30688</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -2366,7 +2375,7 @@
         <v>29007</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -2389,7 +2398,7 @@
         <v>10676</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -2412,7 +2421,7 @@
         <v>8395</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -2435,7 +2444,7 @@
         <v>12340</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -2458,7 +2467,7 @@
         <v>22668</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -2481,7 +2490,7 @@
         <v>37097</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -2504,7 +2513,7 @@
         <v>45454</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -2527,7 +2536,7 @@
         <v>37062</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -2550,7 +2559,7 @@
         <v>27705</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>45</v>
       </c>
@@ -2573,7 +2582,7 @@
         <v>33590</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>45</v>
       </c>
@@ -2596,7 +2605,7 @@
         <v>31968</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>45</v>
       </c>
@@ -2619,7 +2628,7 @@
         <v>17978</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>60</v>
       </c>
@@ -2642,7 +2651,7 @@
         <v>30072</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>60</v>
       </c>
@@ -2665,7 +2674,7 @@
         <v>6682</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>60</v>
       </c>
@@ -2688,7 +2697,7 @@
         <v>27422</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -2711,7 +2720,7 @@
         <v>37097</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -2734,7 +2743,7 @@
         <v>13563</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>60</v>
       </c>
@@ -2757,7 +2766,7 @@
         <v>8721</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>4</v>
       </c>
@@ -2770,8 +2779,18 @@
       <c r="D58" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="E58" s="1">
+        <v>98881.172399999996</v>
+      </c>
+      <c r="F58" s="1">
+        <v>139661.7138</v>
+      </c>
+      <c r="G58" s="1">
+        <v>18340</v>
+      </c>
+      <c r="H58" s="6"/>
+    </row>
+    <row r="59" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>4</v>
       </c>
@@ -2784,8 +2803,17 @@
       <c r="D59" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="E59" s="1">
+        <v>58076.582799999996</v>
+      </c>
+      <c r="F59" s="1">
+        <v>73848.590299999996</v>
+      </c>
+      <c r="G59" s="1">
+        <v>44673</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>4</v>
       </c>
@@ -2798,8 +2826,17 @@
       <c r="D60" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="E60" s="1">
+        <v>35363.476199999997</v>
+      </c>
+      <c r="F60" s="1">
+        <v>51785.846700000002</v>
+      </c>
+      <c r="G60" s="1">
+        <v>37105</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>4</v>
       </c>
@@ -2812,8 +2849,17 @@
       <c r="D61" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="E61" s="1">
+        <v>93173.297000000006</v>
+      </c>
+      <c r="F61" s="1">
+        <v>111385.624</v>
+      </c>
+      <c r="G61" s="1">
+        <v>58442</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>4</v>
       </c>
@@ -2826,8 +2872,17 @@
       <c r="D62" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="E62" s="1">
+        <v>78392.555999999997</v>
+      </c>
+      <c r="F62" s="1">
+        <v>93426.530100000004</v>
+      </c>
+      <c r="G62" s="1">
+        <v>40407</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>4</v>
       </c>
@@ -2840,8 +2895,17 @@
       <c r="D63" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="E63" s="1">
+        <v>99669.231299999999</v>
+      </c>
+      <c r="F63" s="1">
+        <v>144247.85560000001</v>
+      </c>
+      <c r="G63" s="1">
+        <v>27946</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>4</v>
       </c>
@@ -2854,8 +2918,17 @@
       <c r="D64" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E64" s="1">
+        <v>65884.25</v>
+      </c>
+      <c r="F64" s="1">
+        <v>74377.8217</v>
+      </c>
+      <c r="G64" s="1">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>4</v>
       </c>
@@ -2868,8 +2941,17 @@
       <c r="D65" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E65" s="1">
+        <v>82556.337499999994</v>
+      </c>
+      <c r="F65" s="1">
+        <v>106971.9834</v>
+      </c>
+      <c r="G65" s="1">
+        <v>46206</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>4</v>
       </c>
@@ -2882,8 +2964,17 @@
       <c r="D66" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E66" s="1">
+        <v>90529.487800000003</v>
+      </c>
+      <c r="F66" s="1">
+        <v>137945.33850000001</v>
+      </c>
+      <c r="G66" s="1">
+        <v>21077</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>4</v>
       </c>
@@ -2896,8 +2987,17 @@
       <c r="D67" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E67" s="1">
+        <v>53600.332699999999</v>
+      </c>
+      <c r="F67" s="1">
+        <v>77282.489100000006</v>
+      </c>
+      <c r="G67" s="1">
+        <v>12628</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
         <v>4</v>
       </c>
@@ -2910,8 +3010,17 @@
       <c r="D68" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E68" s="5">
+        <v>67705</v>
+      </c>
+      <c r="F68" s="5">
+        <v>99361</v>
+      </c>
+      <c r="G68" s="5">
+        <v>21039</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
         <v>4</v>
       </c>
@@ -2924,8 +3033,17 @@
       <c r="D69" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E69" s="1">
+        <v>55555.897400000002</v>
+      </c>
+      <c r="F69" s="1">
+        <v>69343.763099999996</v>
+      </c>
+      <c r="G69" s="1">
+        <v>26944</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>4</v>
       </c>
@@ -2938,8 +3056,17 @@
       <c r="D70" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E70" s="1">
+        <v>55157.011200000001</v>
+      </c>
+      <c r="F70" s="1">
+        <v>68754.657300000006</v>
+      </c>
+      <c r="G70" s="1">
+        <v>30321</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
         <v>4</v>
       </c>
@@ -2952,8 +3079,17 @@
       <c r="D71" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E71" s="1">
+        <v>58304.0193</v>
+      </c>
+      <c r="F71" s="1">
+        <v>70671.428700000004</v>
+      </c>
+      <c r="G71" s="1">
+        <v>30832</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>9</v>
       </c>
@@ -2966,8 +3102,17 @@
       <c r="D72" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E72" s="1">
+        <v>64804.2264</v>
+      </c>
+      <c r="F72" s="1">
+        <v>79531.967600000004</v>
+      </c>
+      <c r="G72" s="1">
+        <v>21147</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
         <v>9</v>
       </c>
@@ -2980,8 +3125,17 @@
       <c r="D73" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E73" s="1">
+        <v>45265.474999999999</v>
+      </c>
+      <c r="F73" s="1">
+        <v>56202.1921</v>
+      </c>
+      <c r="G73" s="1">
+        <v>23741</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>9</v>
       </c>
@@ -2994,8 +3148,17 @@
       <c r="D74" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E74" s="1">
+        <v>58304.0193</v>
+      </c>
+      <c r="F74" s="1">
+        <v>70671.428700000004</v>
+      </c>
+      <c r="G74" s="1">
+        <v>30832</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>9</v>
       </c>
@@ -3008,8 +3171,17 @@
       <c r="D75" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E75" s="1">
+        <v>76045.592099999994</v>
+      </c>
+      <c r="F75" s="1">
+        <v>93289.298999999999</v>
+      </c>
+      <c r="G75" s="1">
+        <v>17089</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
         <v>9</v>
       </c>
@@ -3022,8 +3194,17 @@
       <c r="D76" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E76" s="1">
+        <v>71692.024600000004</v>
+      </c>
+      <c r="F76" s="1">
+        <v>96371.055800000002</v>
+      </c>
+      <c r="G76" s="1">
+        <v>23586</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
         <v>9</v>
       </c>
@@ -3036,8 +3217,17 @@
       <c r="D77" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E77" s="1">
+        <v>70265.668600000005</v>
+      </c>
+      <c r="F77" s="1">
+        <v>88765.138200000001</v>
+      </c>
+      <c r="G77" s="1">
+        <v>24189</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>9</v>
       </c>
@@ -3050,8 +3240,17 @@
       <c r="D78" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E78" s="1">
+        <v>63322.856099999997</v>
+      </c>
+      <c r="F78" s="1">
+        <v>75211.098899999997</v>
+      </c>
+      <c r="G78" s="1">
+        <v>38290</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
         <v>9</v>
       </c>
@@ -3064,8 +3263,17 @@
       <c r="D79" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E79" s="1">
+        <v>71418.410799999998</v>
+      </c>
+      <c r="F79" s="1">
+        <v>83552.414600000004</v>
+      </c>
+      <c r="G79" s="1">
+        <v>56025</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
         <v>9</v>
       </c>
@@ -3078,8 +3286,17 @@
       <c r="D80" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E80" s="1">
+        <v>68802.7641</v>
+      </c>
+      <c r="F80" s="1">
+        <v>94200.623399999997</v>
+      </c>
+      <c r="G80" s="1">
+        <v>21781</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
         <v>9</v>
       </c>
@@ -3092,8 +3309,17 @@
       <c r="D81" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E81" s="1">
+        <v>128906.2889</v>
+      </c>
+      <c r="F81" s="1">
+        <v>187222.43530000001</v>
+      </c>
+      <c r="G81" s="1">
+        <v>22699</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
         <v>23</v>
       </c>
@@ -3106,8 +3332,17 @@
       <c r="D82" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E82" s="1">
+        <v>51434.857100000001</v>
+      </c>
+      <c r="F82" s="1">
+        <v>66967.746499999994</v>
+      </c>
+      <c r="G82" s="1">
+        <v>27763</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
         <v>23</v>
       </c>
@@ -3120,8 +3355,17 @@
       <c r="D83" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E83" s="1">
+        <v>78699.944499999998</v>
+      </c>
+      <c r="F83" s="1">
+        <v>100868.0583</v>
+      </c>
+      <c r="G83" s="1">
+        <v>27899</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
         <v>23</v>
       </c>
@@ -3134,8 +3378,17 @@
       <c r="D84" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E84" s="1">
+        <v>45355.138500000001</v>
+      </c>
+      <c r="F84" s="1">
+        <v>54362.9758</v>
+      </c>
+      <c r="G84" s="1">
+        <v>31968</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>23</v>
       </c>
@@ -3148,8 +3401,17 @@
       <c r="D85" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E85" s="1">
+        <v>56719.029799999997</v>
+      </c>
+      <c r="F85" s="1">
+        <v>66456.497099999993</v>
+      </c>
+      <c r="G85" s="1">
+        <v>17171</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
         <v>23</v>
       </c>
@@ -3162,8 +3424,17 @@
       <c r="D86" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E86" s="1">
+        <v>74427.105899999995</v>
+      </c>
+      <c r="F86" s="1">
+        <v>91236.916599999997</v>
+      </c>
+      <c r="G86" s="1">
+        <v>26217</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
         <v>23</v>
       </c>
@@ -3176,8 +3447,17 @@
       <c r="D87" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E87" s="1">
+        <v>64848.79</v>
+      </c>
+      <c r="F87" s="1">
+        <v>80240.679799999998</v>
+      </c>
+      <c r="G87" s="1">
+        <v>26168</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
         <v>23</v>
       </c>
@@ -3190,8 +3470,17 @@
       <c r="D88" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E88" s="1">
+        <v>54583.4254</v>
+      </c>
+      <c r="F88" s="1">
+        <v>67917.959600000002</v>
+      </c>
+      <c r="G88" s="1">
+        <v>28896</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
         <v>23</v>
       </c>
@@ -3204,8 +3493,17 @@
       <c r="D89" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E89" s="1">
+        <v>60918.542300000001</v>
+      </c>
+      <c r="F89" s="1">
+        <v>69546.587100000004</v>
+      </c>
+      <c r="G89" s="1">
+        <v>24170</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
         <v>23</v>
       </c>
@@ -3218,8 +3516,17 @@
       <c r="D90" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E90" s="1">
+        <v>62817.184000000001</v>
+      </c>
+      <c r="F90" s="1">
+        <v>74453.195000000007</v>
+      </c>
+      <c r="G90" s="1">
+        <v>45354</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
         <v>23</v>
       </c>
@@ -3232,8 +3539,17 @@
       <c r="D91" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E91" s="1">
+        <v>58400.292399999998</v>
+      </c>
+      <c r="F91" s="1">
+        <v>67613.371400000004</v>
+      </c>
+      <c r="G91" s="1">
+        <v>9703</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
         <v>23</v>
       </c>
@@ -3246,8 +3562,17 @@
       <c r="D92" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E92" s="1">
+        <v>60471.663999999997</v>
+      </c>
+      <c r="F92" s="1">
+        <v>70570.445600000006</v>
+      </c>
+      <c r="G92" s="1">
+        <v>50792</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
         <v>23</v>
       </c>
@@ -3260,8 +3585,17 @@
       <c r="D93" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E93" s="1">
+        <v>42244.986900000004</v>
+      </c>
+      <c r="F93" s="1">
+        <v>57949.0308</v>
+      </c>
+      <c r="G93" s="1">
+        <v>41740</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
         <v>23</v>
       </c>
@@ -3274,8 +3608,17 @@
       <c r="D94" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E94" s="1">
+        <v>58633.131399999998</v>
+      </c>
+      <c r="F94" s="1">
+        <v>64986.597900000001</v>
+      </c>
+      <c r="G94" s="1">
+        <v>11948</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
         <v>23</v>
       </c>
@@ -3288,8 +3631,17 @@
       <c r="D95" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E95" s="1">
+        <v>57182.2189</v>
+      </c>
+      <c r="F95" s="1">
+        <v>71395.290200000003</v>
+      </c>
+      <c r="G95" s="1">
+        <v>44555</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
         <v>23</v>
       </c>
@@ -3302,8 +3654,17 @@
       <c r="D96" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E96" s="1">
+        <v>96608.762000000002</v>
+      </c>
+      <c r="F96" s="1">
+        <v>121401.9497</v>
+      </c>
+      <c r="G96" s="1">
+        <v>34338</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
         <v>23</v>
       </c>
@@ -3316,8 +3677,17 @@
       <c r="D97" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E97" s="1">
+        <v>89013.135899999994</v>
+      </c>
+      <c r="F97" s="1">
+        <v>109566.6116</v>
+      </c>
+      <c r="G97" s="1">
+        <v>24411</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
         <v>23</v>
       </c>
@@ -3330,8 +3700,17 @@
       <c r="D98" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E98" s="1">
+        <v>76908.244900000005</v>
+      </c>
+      <c r="F98" s="1">
+        <v>90008.385699999999</v>
+      </c>
+      <c r="G98" s="1">
+        <v>31365</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
         <v>23</v>
       </c>
@@ -3344,8 +3723,17 @@
       <c r="D99" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E99" s="1">
+        <v>43225.098100000003</v>
+      </c>
+      <c r="F99" s="1">
+        <v>51611.461199999998</v>
+      </c>
+      <c r="G99" s="1">
+        <v>32086</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
         <v>23</v>
       </c>
@@ -3358,8 +3746,17 @@
       <c r="D100" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E100" s="1">
+        <v>52409.904600000002</v>
+      </c>
+      <c r="F100" s="1">
+        <v>63083.267999999996</v>
+      </c>
+      <c r="G100" s="1">
+        <v>44151</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="4" t="s">
         <v>23</v>
       </c>
@@ -3373,7 +3770,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
         <v>23</v>
       </c>
@@ -3387,7 +3784,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="4" t="s">
         <v>23</v>
       </c>
@@ -3401,7 +3798,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
         <v>23</v>
       </c>
@@ -3415,7 +3812,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" s="4" t="s">
         <v>23</v>
       </c>
@@ -3429,7 +3826,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
         <v>23</v>
       </c>
@@ -3443,7 +3840,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" s="4" t="s">
         <v>23</v>
       </c>
@@ -3457,7 +3854,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" s="4" t="s">
         <v>23</v>
       </c>
@@ -3471,7 +3868,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" s="4" t="s">
         <v>23</v>
       </c>
@@ -3485,7 +3882,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" s="4" t="s">
         <v>23</v>
       </c>
@@ -3499,7 +3896,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
         <v>23</v>
       </c>
@@ -3513,7 +3910,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" s="4" t="s">
         <v>23</v>
       </c>
@@ -3527,7 +3924,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="4" t="s">
         <v>23</v>
       </c>
@@ -3541,7 +3938,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="4" t="s">
         <v>23</v>
       </c>
@@ -3555,7 +3952,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="4" t="s">
         <v>23</v>
       </c>
@@ -3569,7 +3966,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="4" t="s">
         <v>23</v>
       </c>
@@ -3583,7 +3980,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="4" t="s">
         <v>23</v>
       </c>
@@ -3597,7 +3994,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="4" t="s">
         <v>23</v>
       </c>
@@ -3611,7 +4008,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" s="4" t="s">
         <v>213</v>
       </c>
@@ -3625,7 +4022,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="4" t="s">
         <v>213</v>
       </c>
@@ -3639,7 +4036,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="4" t="s">
         <v>213</v>
       </c>
@@ -3653,7 +4050,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" s="4" t="s">
         <v>213</v>
       </c>
@@ -3667,7 +4064,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="4" t="s">
         <v>213</v>
       </c>
@@ -3681,7 +4078,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="4" t="s">
         <v>213</v>
       </c>
@@ -3695,7 +4092,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="4" t="s">
         <v>213</v>
       </c>
@@ -3709,7 +4106,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" s="4" t="s">
         <v>213</v>
       </c>
@@ -3723,7 +4120,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" s="4" t="s">
         <v>213</v>
       </c>
@@ -3737,7 +4134,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="4" t="s">
         <v>213</v>
       </c>
@@ -3751,7 +4148,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" s="4" t="s">
         <v>213</v>
       </c>
@@ -3765,7 +4162,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" s="4" t="s">
         <v>213</v>
       </c>
@@ -3779,7 +4176,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" s="4" t="s">
         <v>213</v>
       </c>
@@ -3793,7 +4190,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" s="4" t="s">
         <v>213</v>
       </c>
@@ -3807,7 +4204,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" s="4" t="s">
         <v>213</v>
       </c>
@@ -3821,7 +4218,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" s="4" t="s">
         <v>213</v>
       </c>
@@ -3835,7 +4232,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" s="4" t="s">
         <v>213</v>
       </c>
@@ -3849,7 +4246,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" s="4" t="s">
         <v>213</v>
       </c>
@@ -3863,7 +4260,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" s="4" t="s">
         <v>213</v>
       </c>
@@ -3877,7 +4274,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" s="4" t="s">
         <v>213</v>
       </c>
@@ -3891,7 +4288,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" s="4" t="s">
         <v>213</v>
       </c>
@@ -3905,7 +4302,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" s="4" t="s">
         <v>213</v>
       </c>
@@ -3919,7 +4316,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" s="4" t="s">
         <v>213</v>
       </c>
@@ -3933,7 +4330,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" s="4" t="s">
         <v>213</v>
       </c>
@@ -3947,7 +4344,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" s="4" t="s">
         <v>213</v>
       </c>
@@ -3961,7 +4358,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" s="4" t="s">
         <v>213</v>
       </c>
@@ -3975,7 +4372,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" s="4" t="s">
         <v>213</v>
       </c>
@@ -3989,7 +4386,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" s="4" t="s">
         <v>213</v>
       </c>
@@ -4003,7 +4400,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" s="4" t="s">
         <v>213</v>
       </c>
@@ -4017,7 +4414,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" s="4" t="s">
         <v>213</v>
       </c>
@@ -4031,7 +4428,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" s="4" t="s">
         <v>254</v>
       </c>
@@ -4045,7 +4442,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" s="4" t="s">
         <v>254</v>
       </c>
@@ -4059,7 +4456,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" s="4" t="s">
         <v>254</v>
       </c>
@@ -4073,7 +4470,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" s="4" t="s">
         <v>254</v>
       </c>
@@ -4087,7 +4484,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" s="4" t="s">
         <v>254</v>
       </c>
@@ -4101,7 +4498,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" s="4" t="s">
         <v>34</v>
       </c>
@@ -4115,7 +4512,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" s="4" t="s">
         <v>254</v>
       </c>
@@ -4129,7 +4526,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" s="4" t="s">
         <v>254</v>
       </c>
@@ -4143,7 +4540,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" s="4" t="s">
         <v>254</v>
       </c>
@@ -4157,7 +4554,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="158" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A158" s="4" t="s">
         <v>34</v>
       </c>
@@ -4171,7 +4568,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" s="4" t="s">
         <v>270</v>
       </c>
@@ -4185,7 +4582,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" s="4" t="s">
         <v>270</v>
       </c>
@@ -4199,7 +4596,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" s="4" t="s">
         <v>270</v>
       </c>
@@ -4213,7 +4610,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" s="4" t="s">
         <v>270</v>
       </c>
@@ -4227,7 +4624,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" s="4" t="s">
         <v>270</v>
       </c>
@@ -4241,7 +4638,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" s="4" t="s">
         <v>270</v>
       </c>
@@ -4255,7 +4652,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" s="4" t="s">
         <v>270</v>
       </c>
@@ -4269,7 +4666,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" s="4" t="s">
         <v>270</v>
       </c>
@@ -4283,7 +4680,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" s="4" t="s">
         <v>270</v>
       </c>
@@ -4297,7 +4694,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" s="4" t="s">
         <v>270</v>
       </c>
@@ -4311,7 +4708,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" s="4" t="s">
         <v>270</v>
       </c>
@@ -4325,7 +4722,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" s="4" t="s">
         <v>270</v>
       </c>
@@ -4339,7 +4736,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" s="4" t="s">
         <v>270</v>
       </c>
@@ -4353,7 +4750,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" s="4" t="s">
         <v>270</v>
       </c>
@@ -4367,7 +4764,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" s="4" t="s">
         <v>270</v>
       </c>
@@ -4381,7 +4778,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" s="4" t="s">
         <v>270</v>
       </c>
@@ -4395,7 +4792,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" s="4" t="s">
         <v>270</v>
       </c>
@@ -4409,7 +4806,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" s="4" t="s">
         <v>270</v>
       </c>
@@ -4423,7 +4820,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" s="4" t="s">
         <v>270</v>
       </c>
@@ -4437,7 +4834,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" s="4" t="s">
         <v>270</v>
       </c>
@@ -4451,7 +4848,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="179" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A179" s="4" t="s">
         <v>270</v>
       </c>
@@ -4465,7 +4862,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" s="4" t="s">
         <v>270</v>
       </c>
@@ -4479,7 +4876,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" s="4" t="s">
         <v>270</v>
       </c>
@@ -4493,7 +4890,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" s="4" t="s">
         <v>270</v>
       </c>
@@ -4507,7 +4904,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" s="4" t="s">
         <v>270</v>
       </c>
@@ -4521,7 +4918,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" s="4" t="s">
         <v>270</v>
       </c>
@@ -4535,7 +4932,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" s="4" t="s">
         <v>270</v>
       </c>
@@ -4549,7 +4946,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" s="4" t="s">
         <v>270</v>
       </c>
@@ -4563,7 +4960,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" s="4" t="s">
         <v>60</v>
       </c>
@@ -4577,7 +4974,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" s="4" t="s">
         <v>60</v>
       </c>
@@ -4591,7 +4988,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" s="4" t="s">
         <v>60</v>
       </c>
@@ -4605,7 +5002,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" s="4" t="s">
         <v>60</v>
       </c>
@@ -4619,7 +5016,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" s="4" t="s">
         <v>60</v>
       </c>
@@ -4633,7 +5030,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" s="4" t="s">
         <v>60</v>
       </c>
@@ -4647,7 +5044,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" s="4" t="s">
         <v>60</v>
       </c>
@@ -4661,7 +5058,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" s="4" t="s">
         <v>60</v>
       </c>
@@ -4675,7 +5072,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" s="4" t="s">
         <v>60</v>
       </c>
@@ -4689,7 +5086,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" s="4" t="s">
         <v>60</v>
       </c>
@@ -4703,7 +5100,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" s="4" t="s">
         <v>60</v>
       </c>
@@ -4717,7 +5114,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" s="4" t="s">
         <v>60</v>
       </c>
@@ -4731,7 +5128,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" s="4" t="s">
         <v>60</v>
       </c>
@@ -4745,7 +5142,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" s="4" t="s">
         <v>60</v>
       </c>
@@ -4759,7 +5156,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" s="4" t="s">
         <v>60</v>
       </c>
@@ -4773,7 +5170,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" s="4" t="s">
         <v>60</v>
       </c>
@@ -4787,7 +5184,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203" s="4" t="s">
         <v>60</v>
       </c>
@@ -4801,7 +5198,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204" s="4" t="s">
         <v>60</v>
       </c>
@@ -4815,7 +5212,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" s="4" t="s">
         <v>60</v>
       </c>
@@ -4829,7 +5226,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" s="4" t="s">
         <v>60</v>
       </c>

</xml_diff>

<commit_message>
Add more medium-level stores
</commit_message>
<xml_diff>
--- a/moreWorkingData.xlsx
+++ b/moreWorkingData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mitchell.nguyen/school/senior year/spring 2019/big data/zzz letsGetThisBread/github/LetsGetThisBread/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Navi\Documents\School\CS 438 (Big Data)\LetsGetThisBread\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B165DE6-B9DA-8944-9DAA-0292F410622D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272E4271-27A6-4FD5-A0FE-EF153FD97760}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{224DDC23-A165-FE48-9542-0EB173C9A9C5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25598" windowHeight="15998" xr2:uid="{224DDC23-A165-FE48-9542-0EB173C9A9C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="416">
   <si>
     <t>Grocery Store Name</t>
   </si>
@@ -1065,6 +1065,219 @@
   </si>
   <si>
     <t>5618 Lakewood Town Center Blvd SW, Lakewood, WA 98499</t>
+  </si>
+  <si>
+    <t>1123 Hayden Meadows Drive,  OR 97217</t>
+  </si>
+  <si>
+    <t>2201 Grand Blvd,  WA 98661</t>
+  </si>
+  <si>
+    <t>17275 Nw Cornell Rd,  OR 97006</t>
+  </si>
+  <si>
+    <t>9000 Ne Highway 99,  WA 98665</t>
+  </si>
+  <si>
+    <t>7809 Ne Vancouver Plaza Dr,  WA 98662</t>
+  </si>
+  <si>
+    <t>7650 Ne Shaleen Street,  OR 97006</t>
+  </si>
+  <si>
+    <t>221e Ne 104th Ave,  WA 98664</t>
+  </si>
+  <si>
+    <t>"98664"</t>
+  </si>
+  <si>
+    <t>9055 Sw Murray Blvd,  OR 97008</t>
+  </si>
+  <si>
+    <t>7600 Sw Dartmouth St.,  OR 97223</t>
+  </si>
+  <si>
+    <t>4200 Se 82nd Ave,  OR 97266</t>
+  </si>
+  <si>
+    <t>14505 Ne Fourth Plain Blvd,  WA 98682</t>
+  </si>
+  <si>
+    <t>"98682"</t>
+  </si>
+  <si>
+    <t>430 Se 192nd Ave,  WA 98683</t>
+  </si>
+  <si>
+    <t>10000 Se 82nd Ave,  OR 97086</t>
+  </si>
+  <si>
+    <t>15600 Se Mcloughlin Blvd,  OR 97267</t>
+  </si>
+  <si>
+    <t>1201 Sw 13th Avenue,  WA 98604</t>
+  </si>
+  <si>
+    <t>"98604"</t>
+  </si>
+  <si>
+    <t>19133 Willamette Dr,  OR 97068</t>
+  </si>
+  <si>
+    <t>"97068"</t>
+  </si>
+  <si>
+    <t>220 N Adair St,  OR 97113</t>
+  </si>
+  <si>
+    <t>"97113"</t>
+  </si>
+  <si>
+    <t>3900 W Powell Blvd,  OR 97030</t>
+  </si>
+  <si>
+    <t>21320 Sw Langer Farms Pkwy,  OR 97140</t>
+  </si>
+  <si>
+    <t>"97140"</t>
+  </si>
+  <si>
+    <t>23500 Ne Sandy Blvd,  OR 97060</t>
+  </si>
+  <si>
+    <t>2295 Gable Rd,  OR 97051</t>
+  </si>
+  <si>
+    <t>"97051"</t>
+  </si>
+  <si>
+    <t>2444 E Powell Blvd,  OR 97080</t>
+  </si>
+  <si>
+    <t>1486 Dike Access Rd,  WA 98674</t>
+  </si>
+  <si>
+    <t>3002 Stacey Allison Way,  OR 97071</t>
+  </si>
+  <si>
+    <t>"97071"</t>
+  </si>
+  <si>
+    <t>2375 Ne Highway 99w,  OR 97128</t>
+  </si>
+  <si>
+    <t>540 7th Ave,  WA 98632</t>
+  </si>
+  <si>
+    <t>12620 Se 41st Pl,  WA 98006</t>
+  </si>
+  <si>
+    <t>15063 Main St,  WA 98007</t>
+  </si>
+  <si>
+    <t>743 Rainier Avenue South,  WA 98057</t>
+  </si>
+  <si>
+    <t>6797 State Highway 303 Ne,  WA 98311</t>
+  </si>
+  <si>
+    <t>"98311"</t>
+  </si>
+  <si>
+    <t>3497 Bethel Rd Se,  WA 98366</t>
+  </si>
+  <si>
+    <t>"98366"</t>
+  </si>
+  <si>
+    <t>17222 Highway 99,  WA 98037</t>
+  </si>
+  <si>
+    <t>1900 S 314th St,  WA 98003</t>
+  </si>
+  <si>
+    <t>1400 164th St Sw,  WA 98087</t>
+  </si>
+  <si>
+    <t>"98087"</t>
+  </si>
+  <si>
+    <t>34520 16th Ave S,  WA 98003</t>
+  </si>
+  <si>
+    <t>762 Outlet Collection Way,  WA 98001</t>
+  </si>
+  <si>
+    <t>"98001"</t>
+  </si>
+  <si>
+    <t>21200 Olhava Way Nw,  WA 98370</t>
+  </si>
+  <si>
+    <t>"98370"</t>
+  </si>
+  <si>
+    <t>11400 Highway 99,  WA 98204</t>
+  </si>
+  <si>
+    <t>"98204"</t>
+  </si>
+  <si>
+    <t>1605 Se Everett Mall Way,  WA 98208</t>
+  </si>
+  <si>
+    <t>19191 N Kelsey Street,  WA 98272</t>
+  </si>
+  <si>
+    <t>"98272"</t>
+  </si>
+  <si>
+    <t>1965 S. Union Ave,  WA 98405</t>
+  </si>
+  <si>
+    <t>7001 Bridgeport Way W,  WA 98499</t>
+  </si>
+  <si>
+    <t>310 31st Ave Se,  WA 98374</t>
+  </si>
+  <si>
+    <t>"98374"</t>
+  </si>
+  <si>
+    <t>19205 State Route 410 E,  WA 98391</t>
+  </si>
+  <si>
+    <t>16502 Meridian E,  WA 98375</t>
+  </si>
+  <si>
+    <t>"98375"</t>
+  </si>
+  <si>
+    <t>8713 64th St Ne,  WA 98270</t>
+  </si>
+  <si>
+    <t>"98270"</t>
+  </si>
+  <si>
+    <t>8924 Quilceda Blvd,  WA 98271</t>
+  </si>
+  <si>
+    <t>4010 172nd St Ne,  WA 98223</t>
+  </si>
+  <si>
+    <t>1401 Galaxy Dr Ne,  WA 98516</t>
+  </si>
+  <si>
+    <t>5110 Yelm Highway,  WA 98503</t>
+  </si>
+  <si>
+    <t>"98503"</t>
+  </si>
+  <si>
+    <t>100 E Wallace Kneeland Blvd,  WA 98584</t>
+  </si>
+  <si>
+    <t>"98584"</t>
   </si>
 </sst>
 </file>
@@ -1438,24 +1651,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9739F2B-2F3B-DD45-BA29-3AA82495FC82}">
-  <dimension ref="A1:H206"/>
+  <dimension ref="A1:H257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="75" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView tabSelected="1" topLeftCell="B242" zoomScale="75" workbookViewId="0">
+      <selection activeCell="D257" sqref="D257"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="69.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.8125" customWidth="1"/>
+    <col min="2" max="2" width="12.3125" customWidth="1"/>
+    <col min="3" max="3" width="69.6875" customWidth="1"/>
     <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="25.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="27.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.6875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.1875" style="1" customWidth="1"/>
     <col min="7" max="7" width="22" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1478,7 +1691,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1501,7 +1714,7 @@
         <v>23200</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1524,7 +1737,7 @@
         <v>29007</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1547,7 +1760,7 @@
         <v>22668</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1570,7 +1783,7 @@
         <v>8395</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1593,7 +1806,7 @@
         <v>27612</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1616,7 +1829,7 @@
         <v>30072</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1639,7 +1852,7 @@
         <v>9915</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1662,7 +1875,7 @@
         <v>23200</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1685,7 +1898,7 @@
         <v>30688</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1708,7 +1921,7 @@
         <v>10676</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1731,7 +1944,7 @@
         <v>22668</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1754,7 +1967,7 @@
         <v>37097</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1777,7 +1990,7 @@
         <v>45454</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -1800,7 +2013,7 @@
         <v>37097</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1823,7 +2036,7 @@
         <v>30072</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1846,7 +2059,7 @@
         <v>28254</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1869,7 +2082,7 @@
         <v>17978</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1892,7 +2105,7 @@
         <v>27612</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1915,7 +2128,7 @@
         <v>29007</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -1938,7 +2151,7 @@
         <v>45454</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1961,7 +2174,7 @@
         <v>28254</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1984,7 +2197,7 @@
         <v>27422</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -2007,7 +2220,7 @@
         <v>31968</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -2030,7 +2243,7 @@
         <v>30072</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -2053,7 +2266,7 @@
         <v>12340</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -2076,7 +2289,7 @@
         <v>10676</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -2099,7 +2312,7 @@
         <v>27612</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -2122,7 +2335,7 @@
         <v>30072</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -2145,7 +2358,7 @@
         <v>8395</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -2168,7 +2381,7 @@
         <v>10676</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -2191,7 +2404,7 @@
         <v>37062</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -2214,7 +2427,7 @@
         <v>22668</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -2237,7 +2450,7 @@
         <v>29007</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -2260,7 +2473,7 @@
         <v>27422</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -2283,7 +2496,7 @@
         <v>27705</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -2306,7 +2519,7 @@
         <v>17978</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
         <v>45</v>
       </c>
@@ -2329,7 +2542,7 @@
         <v>27612</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -2352,7 +2565,7 @@
         <v>30688</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -2375,7 +2588,7 @@
         <v>29007</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -2398,7 +2611,7 @@
         <v>10676</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -2421,7 +2634,7 @@
         <v>8395</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -2444,7 +2657,7 @@
         <v>12340</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -2467,7 +2680,7 @@
         <v>22668</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -2490,7 +2703,7 @@
         <v>37097</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -2513,7 +2726,7 @@
         <v>45454</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -2536,7 +2749,7 @@
         <v>37062</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -2559,7 +2772,7 @@
         <v>27705</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A49" t="s">
         <v>45</v>
       </c>
@@ -2582,7 +2795,7 @@
         <v>33590</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A50" t="s">
         <v>45</v>
       </c>
@@ -2605,7 +2818,7 @@
         <v>31968</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A51" t="s">
         <v>45</v>
       </c>
@@ -2628,7 +2841,7 @@
         <v>17978</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A52" t="s">
         <v>60</v>
       </c>
@@ -2651,7 +2864,7 @@
         <v>30072</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A53" t="s">
         <v>60</v>
       </c>
@@ -2674,7 +2887,7 @@
         <v>6682</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A54" t="s">
         <v>60</v>
       </c>
@@ -2697,7 +2910,7 @@
         <v>27422</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -2720,7 +2933,7 @@
         <v>37097</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -2743,7 +2956,7 @@
         <v>13563</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A57" t="s">
         <v>60</v>
       </c>
@@ -2766,7 +2979,7 @@
         <v>8721</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A58" t="s">
         <v>4</v>
       </c>
@@ -2790,7 +3003,7 @@
       </c>
       <c r="H58" s="6"/>
     </row>
-    <row r="59" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A59" t="s">
         <v>4</v>
       </c>
@@ -2813,7 +3026,7 @@
         <v>44673</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A60" t="s">
         <v>4</v>
       </c>
@@ -2836,7 +3049,7 @@
         <v>37105</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A61" s="4" t="s">
         <v>4</v>
       </c>
@@ -2859,7 +3072,7 @@
         <v>58442</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A62" s="4" t="s">
         <v>4</v>
       </c>
@@ -2882,7 +3095,7 @@
         <v>40407</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A63" s="4" t="s">
         <v>4</v>
       </c>
@@ -2905,7 +3118,7 @@
         <v>27946</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A64" s="4" t="s">
         <v>4</v>
       </c>
@@ -2928,7 +3141,7 @@
         <v>36000</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A65" s="4" t="s">
         <v>4</v>
       </c>
@@ -2951,7 +3164,7 @@
         <v>46206</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A66" s="4" t="s">
         <v>4</v>
       </c>
@@ -2974,7 +3187,7 @@
         <v>21077</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A67" s="4" t="s">
         <v>4</v>
       </c>
@@ -2997,7 +3210,7 @@
         <v>12628</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A68" s="4" t="s">
         <v>4</v>
       </c>
@@ -3020,7 +3233,7 @@
         <v>21039</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A69" s="4" t="s">
         <v>4</v>
       </c>
@@ -3043,7 +3256,7 @@
         <v>26944</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A70" s="4" t="s">
         <v>4</v>
       </c>
@@ -3066,7 +3279,7 @@
         <v>30321</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A71" s="4" t="s">
         <v>4</v>
       </c>
@@ -3089,7 +3302,7 @@
         <v>30832</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A72" s="4" t="s">
         <v>9</v>
       </c>
@@ -3112,7 +3325,7 @@
         <v>21147</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A73" s="4" t="s">
         <v>9</v>
       </c>
@@ -3135,7 +3348,7 @@
         <v>23741</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A74" s="4" t="s">
         <v>9</v>
       </c>
@@ -3158,7 +3371,7 @@
         <v>30832</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A75" s="4" t="s">
         <v>9</v>
       </c>
@@ -3181,7 +3394,7 @@
         <v>17089</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A76" s="4" t="s">
         <v>9</v>
       </c>
@@ -3204,7 +3417,7 @@
         <v>23586</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A77" s="4" t="s">
         <v>9</v>
       </c>
@@ -3227,7 +3440,7 @@
         <v>24189</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A78" s="4" t="s">
         <v>9</v>
       </c>
@@ -3250,7 +3463,7 @@
         <v>38290</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A79" s="4" t="s">
         <v>9</v>
       </c>
@@ -3273,7 +3486,7 @@
         <v>56025</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A80" s="4" t="s">
         <v>9</v>
       </c>
@@ -3296,7 +3509,7 @@
         <v>21781</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A81" s="4" t="s">
         <v>9</v>
       </c>
@@ -3319,7 +3532,7 @@
         <v>22699</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A82" s="4" t="s">
         <v>23</v>
       </c>
@@ -3342,7 +3555,7 @@
         <v>27763</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A83" s="4" t="s">
         <v>23</v>
       </c>
@@ -3365,7 +3578,7 @@
         <v>27899</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A84" s="4" t="s">
         <v>23</v>
       </c>
@@ -3388,7 +3601,7 @@
         <v>31968</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A85" s="4" t="s">
         <v>23</v>
       </c>
@@ -3411,7 +3624,7 @@
         <v>17171</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A86" s="4" t="s">
         <v>23</v>
       </c>
@@ -3434,7 +3647,7 @@
         <v>26217</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A87" s="4" t="s">
         <v>23</v>
       </c>
@@ -3457,7 +3670,7 @@
         <v>26168</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A88" s="4" t="s">
         <v>23</v>
       </c>
@@ -3480,7 +3693,7 @@
         <v>28896</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A89" s="4" t="s">
         <v>23</v>
       </c>
@@ -3503,7 +3716,7 @@
         <v>24170</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A90" s="4" t="s">
         <v>23</v>
       </c>
@@ -3526,7 +3739,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A91" s="4" t="s">
         <v>23</v>
       </c>
@@ -3549,7 +3762,7 @@
         <v>9703</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A92" s="4" t="s">
         <v>23</v>
       </c>
@@ -3572,7 +3785,7 @@
         <v>50792</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A93" s="4" t="s">
         <v>23</v>
       </c>
@@ -3595,7 +3808,7 @@
         <v>41740</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A94" s="4" t="s">
         <v>23</v>
       </c>
@@ -3618,7 +3831,7 @@
         <v>11948</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A95" s="4" t="s">
         <v>23</v>
       </c>
@@ -3641,7 +3854,7 @@
         <v>44555</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A96" s="4" t="s">
         <v>23</v>
       </c>
@@ -3664,7 +3877,7 @@
         <v>34338</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A97" s="4" t="s">
         <v>23</v>
       </c>
@@ -3687,7 +3900,7 @@
         <v>24411</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A98" s="4" t="s">
         <v>23</v>
       </c>
@@ -3710,7 +3923,7 @@
         <v>31365</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A99" s="4" t="s">
         <v>23</v>
       </c>
@@ -3733,7 +3946,7 @@
         <v>32086</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A100" s="4" t="s">
         <v>23</v>
       </c>
@@ -3756,7 +3969,7 @@
         <v>44151</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A101" s="4" t="s">
         <v>23</v>
       </c>
@@ -3770,7 +3983,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A102" s="4" t="s">
         <v>23</v>
       </c>
@@ -3784,7 +3997,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A103" s="4" t="s">
         <v>23</v>
       </c>
@@ -3798,7 +4011,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A104" s="4" t="s">
         <v>23</v>
       </c>
@@ -3812,7 +4025,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A105" s="4" t="s">
         <v>23</v>
       </c>
@@ -3826,7 +4039,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A106" s="4" t="s">
         <v>23</v>
       </c>
@@ -3840,7 +4053,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A107" s="4" t="s">
         <v>23</v>
       </c>
@@ -3854,7 +4067,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A108" s="4" t="s">
         <v>23</v>
       </c>
@@ -3868,7 +4081,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A109" s="4" t="s">
         <v>23</v>
       </c>
@@ -3882,7 +4095,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A110" s="4" t="s">
         <v>23</v>
       </c>
@@ -3896,7 +4109,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A111" s="4" t="s">
         <v>23</v>
       </c>
@@ -3910,7 +4123,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A112" s="4" t="s">
         <v>23</v>
       </c>
@@ -3924,7 +4137,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A113" s="4" t="s">
         <v>23</v>
       </c>
@@ -3938,7 +4151,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A114" s="4" t="s">
         <v>23</v>
       </c>
@@ -3952,7 +4165,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A115" s="4" t="s">
         <v>23</v>
       </c>
@@ -3966,7 +4179,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A116" s="4" t="s">
         <v>23</v>
       </c>
@@ -3980,7 +4193,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A117" s="4" t="s">
         <v>23</v>
       </c>
@@ -3994,7 +4207,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A118" s="4" t="s">
         <v>23</v>
       </c>
@@ -4008,7 +4221,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A119" s="4" t="s">
         <v>213</v>
       </c>
@@ -4022,7 +4235,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A120" s="4" t="s">
         <v>213</v>
       </c>
@@ -4036,7 +4249,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A121" s="4" t="s">
         <v>213</v>
       </c>
@@ -4050,7 +4263,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A122" s="4" t="s">
         <v>213</v>
       </c>
@@ -4064,7 +4277,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A123" s="4" t="s">
         <v>213</v>
       </c>
@@ -4078,7 +4291,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A124" s="4" t="s">
         <v>213</v>
       </c>
@@ -4092,7 +4305,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A125" s="4" t="s">
         <v>213</v>
       </c>
@@ -4106,7 +4319,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A126" s="4" t="s">
         <v>213</v>
       </c>
@@ -4120,7 +4333,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A127" s="4" t="s">
         <v>213</v>
       </c>
@@ -4134,7 +4347,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A128" s="4" t="s">
         <v>213</v>
       </c>
@@ -4148,7 +4361,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A129" s="4" t="s">
         <v>213</v>
       </c>
@@ -4162,7 +4375,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A130" s="4" t="s">
         <v>213</v>
       </c>
@@ -4176,7 +4389,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A131" s="4" t="s">
         <v>213</v>
       </c>
@@ -4190,7 +4403,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A132" s="4" t="s">
         <v>213</v>
       </c>
@@ -4204,7 +4417,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A133" s="4" t="s">
         <v>213</v>
       </c>
@@ -4218,7 +4431,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A134" s="4" t="s">
         <v>213</v>
       </c>
@@ -4232,7 +4445,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A135" s="4" t="s">
         <v>213</v>
       </c>
@@ -4246,7 +4459,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A136" s="4" t="s">
         <v>213</v>
       </c>
@@ -4260,7 +4473,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A137" s="4" t="s">
         <v>213</v>
       </c>
@@ -4274,7 +4487,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A138" s="4" t="s">
         <v>213</v>
       </c>
@@ -4288,7 +4501,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A139" s="4" t="s">
         <v>213</v>
       </c>
@@ -4302,7 +4515,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A140" s="4" t="s">
         <v>213</v>
       </c>
@@ -4316,7 +4529,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A141" s="4" t="s">
         <v>213</v>
       </c>
@@ -4330,7 +4543,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A142" s="4" t="s">
         <v>213</v>
       </c>
@@ -4344,7 +4557,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A143" s="4" t="s">
         <v>213</v>
       </c>
@@ -4358,7 +4571,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A144" s="4" t="s">
         <v>213</v>
       </c>
@@ -4372,7 +4585,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A145" s="4" t="s">
         <v>213</v>
       </c>
@@ -4386,7 +4599,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A146" s="4" t="s">
         <v>213</v>
       </c>
@@ -4400,7 +4613,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A147" s="4" t="s">
         <v>213</v>
       </c>
@@ -4414,7 +4627,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A148" s="4" t="s">
         <v>213</v>
       </c>
@@ -4428,7 +4641,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A149" s="4" t="s">
         <v>254</v>
       </c>
@@ -4442,7 +4655,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A150" s="4" t="s">
         <v>254</v>
       </c>
@@ -4456,7 +4669,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A151" s="4" t="s">
         <v>254</v>
       </c>
@@ -4470,7 +4683,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A152" s="4" t="s">
         <v>254</v>
       </c>
@@ -4484,7 +4697,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A153" s="4" t="s">
         <v>254</v>
       </c>
@@ -4498,7 +4711,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A154" s="4" t="s">
         <v>34</v>
       </c>
@@ -4512,7 +4725,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A155" s="4" t="s">
         <v>254</v>
       </c>
@@ -4526,7 +4739,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A156" s="4" t="s">
         <v>254</v>
       </c>
@@ -4540,7 +4753,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A157" s="4" t="s">
         <v>254</v>
       </c>
@@ -4554,7 +4767,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A158" s="4" t="s">
         <v>34</v>
       </c>
@@ -4568,7 +4781,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A159" s="4" t="s">
         <v>270</v>
       </c>
@@ -4582,7 +4795,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A160" s="4" t="s">
         <v>270</v>
       </c>
@@ -4596,7 +4809,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A161" s="4" t="s">
         <v>270</v>
       </c>
@@ -4610,7 +4823,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A162" s="4" t="s">
         <v>270</v>
       </c>
@@ -4624,7 +4837,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A163" s="4" t="s">
         <v>270</v>
       </c>
@@ -4638,7 +4851,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A164" s="4" t="s">
         <v>270</v>
       </c>
@@ -4652,7 +4865,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A165" s="4" t="s">
         <v>270</v>
       </c>
@@ -4666,7 +4879,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A166" s="4" t="s">
         <v>270</v>
       </c>
@@ -4680,7 +4893,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A167" s="4" t="s">
         <v>270</v>
       </c>
@@ -4694,7 +4907,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A168" s="4" t="s">
         <v>270</v>
       </c>
@@ -4708,7 +4921,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A169" s="4" t="s">
         <v>270</v>
       </c>
@@ -4722,7 +4935,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A170" s="4" t="s">
         <v>270</v>
       </c>
@@ -4736,7 +4949,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A171" s="4" t="s">
         <v>270</v>
       </c>
@@ -4750,7 +4963,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A172" s="4" t="s">
         <v>270</v>
       </c>
@@ -4764,7 +4977,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A173" s="4" t="s">
         <v>270</v>
       </c>
@@ -4778,7 +4991,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A174" s="4" t="s">
         <v>270</v>
       </c>
@@ -4792,7 +5005,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A175" s="4" t="s">
         <v>270</v>
       </c>
@@ -4806,7 +5019,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A176" s="4" t="s">
         <v>270</v>
       </c>
@@ -4820,7 +5033,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A177" s="4" t="s">
         <v>270</v>
       </c>
@@ -4834,7 +5047,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A178" s="4" t="s">
         <v>270</v>
       </c>
@@ -4848,7 +5061,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="179" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A179" s="4" t="s">
         <v>270</v>
       </c>
@@ -4862,7 +5075,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A180" s="4" t="s">
         <v>270</v>
       </c>
@@ -4876,7 +5089,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A181" s="4" t="s">
         <v>270</v>
       </c>
@@ -4890,7 +5103,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A182" s="4" t="s">
         <v>270</v>
       </c>
@@ -4904,7 +5117,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A183" s="4" t="s">
         <v>270</v>
       </c>
@@ -4918,7 +5131,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A184" s="4" t="s">
         <v>270</v>
       </c>
@@ -4932,7 +5145,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A185" s="4" t="s">
         <v>270</v>
       </c>
@@ -4946,7 +5159,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A186" s="4" t="s">
         <v>270</v>
       </c>
@@ -4960,7 +5173,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A187" s="4" t="s">
         <v>60</v>
       </c>
@@ -4974,7 +5187,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A188" s="4" t="s">
         <v>60</v>
       </c>
@@ -4988,7 +5201,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A189" s="4" t="s">
         <v>60</v>
       </c>
@@ -5002,7 +5215,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A190" s="4" t="s">
         <v>60</v>
       </c>
@@ -5016,7 +5229,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A191" s="4" t="s">
         <v>60</v>
       </c>
@@ -5030,7 +5243,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A192" s="4" t="s">
         <v>60</v>
       </c>
@@ -5044,7 +5257,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A193" s="4" t="s">
         <v>60</v>
       </c>
@@ -5058,7 +5271,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A194" s="4" t="s">
         <v>60</v>
       </c>
@@ -5072,7 +5285,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A195" s="4" t="s">
         <v>60</v>
       </c>
@@ -5086,7 +5299,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A196" s="4" t="s">
         <v>60</v>
       </c>
@@ -5100,7 +5313,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A197" s="4" t="s">
         <v>60</v>
       </c>
@@ -5114,7 +5327,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A198" s="4" t="s">
         <v>60</v>
       </c>
@@ -5128,7 +5341,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A199" s="4" t="s">
         <v>60</v>
       </c>
@@ -5142,7 +5355,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A200" s="4" t="s">
         <v>60</v>
       </c>
@@ -5156,7 +5369,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A201" s="4" t="s">
         <v>60</v>
       </c>
@@ -5170,7 +5383,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A202" s="4" t="s">
         <v>60</v>
       </c>
@@ -5184,7 +5397,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A203" s="4" t="s">
         <v>60</v>
       </c>
@@ -5198,7 +5411,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A204" s="4" t="s">
         <v>60</v>
       </c>
@@ -5212,7 +5425,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A205" s="4" t="s">
         <v>60</v>
       </c>
@@ -5226,7 +5439,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A206" s="4" t="s">
         <v>60</v>
       </c>
@@ -5238,6 +5451,720 @@
       </c>
       <c r="D206" t="s">
         <v>191</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A207" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B207">
+        <v>2</v>
+      </c>
+      <c r="C207" t="s">
+        <v>345</v>
+      </c>
+      <c r="D207" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A208" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B208">
+        <v>2</v>
+      </c>
+      <c r="C208" t="s">
+        <v>346</v>
+      </c>
+      <c r="D208" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A209" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B209">
+        <v>2</v>
+      </c>
+      <c r="C209" t="s">
+        <v>347</v>
+      </c>
+      <c r="D209" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A210" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B210">
+        <v>2</v>
+      </c>
+      <c r="C210" t="s">
+        <v>348</v>
+      </c>
+      <c r="D210" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A211" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B211">
+        <v>2</v>
+      </c>
+      <c r="C211" t="s">
+        <v>349</v>
+      </c>
+      <c r="D211" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A212" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B212">
+        <v>2</v>
+      </c>
+      <c r="C212" t="s">
+        <v>350</v>
+      </c>
+      <c r="D212" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A213" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B213">
+        <v>2</v>
+      </c>
+      <c r="C213" t="s">
+        <v>351</v>
+      </c>
+      <c r="D213" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A214" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B214">
+        <v>2</v>
+      </c>
+      <c r="C214" t="s">
+        <v>353</v>
+      </c>
+      <c r="D214" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A215" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B215">
+        <v>2</v>
+      </c>
+      <c r="C215" t="s">
+        <v>354</v>
+      </c>
+      <c r="D215" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A216" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B216">
+        <v>2</v>
+      </c>
+      <c r="C216" t="s">
+        <v>355</v>
+      </c>
+      <c r="D216" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A217" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B217">
+        <v>2</v>
+      </c>
+      <c r="C217" t="s">
+        <v>356</v>
+      </c>
+      <c r="D217" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A218" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B218">
+        <v>2</v>
+      </c>
+      <c r="C218" t="s">
+        <v>358</v>
+      </c>
+      <c r="D218" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A219" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B219">
+        <v>2</v>
+      </c>
+      <c r="C219" t="s">
+        <v>359</v>
+      </c>
+      <c r="D219" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A220" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B220">
+        <v>2</v>
+      </c>
+      <c r="C220" t="s">
+        <v>360</v>
+      </c>
+      <c r="D220" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A221" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B221">
+        <v>2</v>
+      </c>
+      <c r="C221" t="s">
+        <v>361</v>
+      </c>
+      <c r="D221" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A222" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B222">
+        <v>2</v>
+      </c>
+      <c r="C222" t="s">
+        <v>363</v>
+      </c>
+      <c r="D222" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A223" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B223">
+        <v>2</v>
+      </c>
+      <c r="C223" t="s">
+        <v>365</v>
+      </c>
+      <c r="D223" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A224" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B224">
+        <v>2</v>
+      </c>
+      <c r="C224" t="s">
+        <v>367</v>
+      </c>
+      <c r="D224" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A225" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B225">
+        <v>2</v>
+      </c>
+      <c r="C225" t="s">
+        <v>368</v>
+      </c>
+      <c r="D225" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A226" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B226">
+        <v>2</v>
+      </c>
+      <c r="C226" t="s">
+        <v>370</v>
+      </c>
+      <c r="D226" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A227" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B227">
+        <v>2</v>
+      </c>
+      <c r="C227" t="s">
+        <v>371</v>
+      </c>
+      <c r="D227" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A228" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B228">
+        <v>2</v>
+      </c>
+      <c r="C228" t="s">
+        <v>373</v>
+      </c>
+      <c r="D228" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A229" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B229">
+        <v>2</v>
+      </c>
+      <c r="C229" t="s">
+        <v>374</v>
+      </c>
+      <c r="D229" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A230" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B230">
+        <v>2</v>
+      </c>
+      <c r="C230" t="s">
+        <v>375</v>
+      </c>
+      <c r="D230" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A231" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B231">
+        <v>2</v>
+      </c>
+      <c r="C231" t="s">
+        <v>377</v>
+      </c>
+      <c r="D231" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A232" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B232">
+        <v>2</v>
+      </c>
+      <c r="C232" t="s">
+        <v>378</v>
+      </c>
+      <c r="D232" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A233" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B233">
+        <v>2</v>
+      </c>
+      <c r="C233" t="s">
+        <v>379</v>
+      </c>
+      <c r="D233" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A234" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B234">
+        <v>2</v>
+      </c>
+      <c r="C234" t="s">
+        <v>380</v>
+      </c>
+      <c r="D234" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A235" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B235">
+        <v>2</v>
+      </c>
+      <c r="C235" t="s">
+        <v>381</v>
+      </c>
+      <c r="D235" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A236" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B236">
+        <v>2</v>
+      </c>
+      <c r="C236" t="s">
+        <v>382</v>
+      </c>
+      <c r="D236" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A237" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B237">
+        <v>2</v>
+      </c>
+      <c r="C237" t="s">
+        <v>384</v>
+      </c>
+      <c r="D237" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A238" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B238">
+        <v>2</v>
+      </c>
+      <c r="C238" t="s">
+        <v>386</v>
+      </c>
+      <c r="D238" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A239" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B239">
+        <v>2</v>
+      </c>
+      <c r="C239" t="s">
+        <v>387</v>
+      </c>
+      <c r="D239" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A240" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B240">
+        <v>2</v>
+      </c>
+      <c r="C240" t="s">
+        <v>388</v>
+      </c>
+      <c r="D240" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A241" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B241">
+        <v>2</v>
+      </c>
+      <c r="C241" t="s">
+        <v>390</v>
+      </c>
+      <c r="D241" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A242" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B242">
+        <v>2</v>
+      </c>
+      <c r="C242" t="s">
+        <v>391</v>
+      </c>
+      <c r="D242" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A243" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B243">
+        <v>2</v>
+      </c>
+      <c r="C243" t="s">
+        <v>393</v>
+      </c>
+      <c r="D243" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A244" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B244">
+        <v>2</v>
+      </c>
+      <c r="C244" t="s">
+        <v>395</v>
+      </c>
+      <c r="D244" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A245" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B245">
+        <v>2</v>
+      </c>
+      <c r="C245" t="s">
+        <v>397</v>
+      </c>
+      <c r="D245" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A246" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B246">
+        <v>2</v>
+      </c>
+      <c r="C246" t="s">
+        <v>398</v>
+      </c>
+      <c r="D246" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A247" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B247">
+        <v>2</v>
+      </c>
+      <c r="C247" t="s">
+        <v>400</v>
+      </c>
+      <c r="D247" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A248" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B248">
+        <v>2</v>
+      </c>
+      <c r="C248" t="s">
+        <v>401</v>
+      </c>
+      <c r="D248" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A249" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B249">
+        <v>2</v>
+      </c>
+      <c r="C249" t="s">
+        <v>402</v>
+      </c>
+      <c r="D249" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A250" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B250">
+        <v>2</v>
+      </c>
+      <c r="C250" t="s">
+        <v>404</v>
+      </c>
+      <c r="D250" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A251" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B251">
+        <v>2</v>
+      </c>
+      <c r="C251" t="s">
+        <v>405</v>
+      </c>
+      <c r="D251" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A252" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B252">
+        <v>2</v>
+      </c>
+      <c r="C252" t="s">
+        <v>407</v>
+      </c>
+      <c r="D252" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A253" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B253">
+        <v>2</v>
+      </c>
+      <c r="C253" t="s">
+        <v>409</v>
+      </c>
+      <c r="D253" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A254" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B254">
+        <v>2</v>
+      </c>
+      <c r="C254" t="s">
+        <v>410</v>
+      </c>
+      <c r="D254" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A255" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B255">
+        <v>2</v>
+      </c>
+      <c r="C255" t="s">
+        <v>411</v>
+      </c>
+      <c r="D255" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A256" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B256">
+        <v>2</v>
+      </c>
+      <c r="C256" t="s">
+        <v>412</v>
+      </c>
+      <c r="D256" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A257" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B257">
+        <v>2</v>
+      </c>
+      <c r="C257" t="s">
+        <v>414</v>
+      </c>
+      <c r="D257" t="s">
+        <v>415</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix classifications of stores
</commit_message>
<xml_diff>
--- a/moreWorkingData.xlsx
+++ b/moreWorkingData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Navi\Documents\School\CS 438 (Big Data)\LetsGetThisBread\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272E4271-27A6-4FD5-A0FE-EF153FD97760}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF3CC79-D7D6-4872-B533-91B8B5363CE2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25598" windowHeight="15998" xr2:uid="{224DDC23-A165-FE48-9542-0EB173C9A9C5}"/>
   </bookViews>
@@ -1653,8 +1653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9739F2B-2F3B-DD45-BA29-3AA82495FC82}">
   <dimension ref="A1:H257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B242" zoomScale="75" workbookViewId="0">
-      <selection activeCell="D257" sqref="D257"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="75" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -5458,7 +5458,7 @@
         <v>19</v>
       </c>
       <c r="B207">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C207" t="s">
         <v>345</v>
@@ -5472,7 +5472,7 @@
         <v>19</v>
       </c>
       <c r="B208">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C208" t="s">
         <v>346</v>
@@ -5486,7 +5486,7 @@
         <v>19</v>
       </c>
       <c r="B209">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C209" t="s">
         <v>347</v>
@@ -5500,7 +5500,7 @@
         <v>19</v>
       </c>
       <c r="B210">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C210" t="s">
         <v>348</v>
@@ -5514,7 +5514,7 @@
         <v>19</v>
       </c>
       <c r="B211">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C211" t="s">
         <v>349</v>
@@ -5528,7 +5528,7 @@
         <v>19</v>
       </c>
       <c r="B212">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C212" t="s">
         <v>350</v>
@@ -5542,7 +5542,7 @@
         <v>19</v>
       </c>
       <c r="B213">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C213" t="s">
         <v>351</v>
@@ -5556,7 +5556,7 @@
         <v>19</v>
       </c>
       <c r="B214">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C214" t="s">
         <v>353</v>
@@ -5570,7 +5570,7 @@
         <v>19</v>
       </c>
       <c r="B215">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C215" t="s">
         <v>354</v>
@@ -5584,7 +5584,7 @@
         <v>19</v>
       </c>
       <c r="B216">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C216" t="s">
         <v>355</v>
@@ -5598,7 +5598,7 @@
         <v>19</v>
       </c>
       <c r="B217">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C217" t="s">
         <v>356</v>
@@ -5612,7 +5612,7 @@
         <v>19</v>
       </c>
       <c r="B218">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C218" t="s">
         <v>358</v>
@@ -5626,7 +5626,7 @@
         <v>19</v>
       </c>
       <c r="B219">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C219" t="s">
         <v>359</v>
@@ -5640,7 +5640,7 @@
         <v>19</v>
       </c>
       <c r="B220">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C220" t="s">
         <v>360</v>
@@ -5654,7 +5654,7 @@
         <v>19</v>
       </c>
       <c r="B221">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C221" t="s">
         <v>361</v>
@@ -5668,7 +5668,7 @@
         <v>19</v>
       </c>
       <c r="B222">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C222" t="s">
         <v>363</v>
@@ -5682,7 +5682,7 @@
         <v>19</v>
       </c>
       <c r="B223">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C223" t="s">
         <v>365</v>
@@ -5696,7 +5696,7 @@
         <v>19</v>
       </c>
       <c r="B224">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C224" t="s">
         <v>367</v>
@@ -5710,7 +5710,7 @@
         <v>19</v>
       </c>
       <c r="B225">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C225" t="s">
         <v>368</v>
@@ -5724,7 +5724,7 @@
         <v>19</v>
       </c>
       <c r="B226">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C226" t="s">
         <v>370</v>
@@ -5738,7 +5738,7 @@
         <v>19</v>
       </c>
       <c r="B227">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C227" t="s">
         <v>371</v>
@@ -5752,7 +5752,7 @@
         <v>19</v>
       </c>
       <c r="B228">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C228" t="s">
         <v>373</v>
@@ -5766,7 +5766,7 @@
         <v>19</v>
       </c>
       <c r="B229">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C229" t="s">
         <v>374</v>
@@ -5780,7 +5780,7 @@
         <v>19</v>
       </c>
       <c r="B230">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C230" t="s">
         <v>375</v>
@@ -5794,7 +5794,7 @@
         <v>19</v>
       </c>
       <c r="B231">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C231" t="s">
         <v>377</v>
@@ -5808,7 +5808,7 @@
         <v>19</v>
       </c>
       <c r="B232">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C232" t="s">
         <v>378</v>
@@ -5822,7 +5822,7 @@
         <v>19</v>
       </c>
       <c r="B233">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C233" t="s">
         <v>379</v>
@@ -5836,7 +5836,7 @@
         <v>19</v>
       </c>
       <c r="B234">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C234" t="s">
         <v>380</v>
@@ -5850,7 +5850,7 @@
         <v>19</v>
       </c>
       <c r="B235">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C235" t="s">
         <v>381</v>
@@ -5864,7 +5864,7 @@
         <v>19</v>
       </c>
       <c r="B236">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C236" t="s">
         <v>382</v>
@@ -5878,7 +5878,7 @@
         <v>19</v>
       </c>
       <c r="B237">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C237" t="s">
         <v>384</v>
@@ -5892,7 +5892,7 @@
         <v>19</v>
       </c>
       <c r="B238">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C238" t="s">
         <v>386</v>
@@ -5906,7 +5906,7 @@
         <v>19</v>
       </c>
       <c r="B239">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C239" t="s">
         <v>387</v>
@@ -5920,7 +5920,7 @@
         <v>19</v>
       </c>
       <c r="B240">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C240" t="s">
         <v>388</v>
@@ -5934,7 +5934,7 @@
         <v>19</v>
       </c>
       <c r="B241">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C241" t="s">
         <v>390</v>
@@ -5948,7 +5948,7 @@
         <v>19</v>
       </c>
       <c r="B242">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C242" t="s">
         <v>391</v>
@@ -5962,7 +5962,7 @@
         <v>19</v>
       </c>
       <c r="B243">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C243" t="s">
         <v>393</v>
@@ -5976,7 +5976,7 @@
         <v>19</v>
       </c>
       <c r="B244">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C244" t="s">
         <v>395</v>
@@ -5990,7 +5990,7 @@
         <v>19</v>
       </c>
       <c r="B245">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C245" t="s">
         <v>397</v>
@@ -6004,7 +6004,7 @@
         <v>19</v>
       </c>
       <c r="B246">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C246" t="s">
         <v>398</v>
@@ -6018,7 +6018,7 @@
         <v>19</v>
       </c>
       <c r="B247">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C247" t="s">
         <v>400</v>
@@ -6032,7 +6032,7 @@
         <v>19</v>
       </c>
       <c r="B248">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C248" t="s">
         <v>401</v>
@@ -6046,7 +6046,7 @@
         <v>19</v>
       </c>
       <c r="B249">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C249" t="s">
         <v>402</v>
@@ -6060,7 +6060,7 @@
         <v>19</v>
       </c>
       <c r="B250">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C250" t="s">
         <v>404</v>
@@ -6074,7 +6074,7 @@
         <v>19</v>
       </c>
       <c r="B251">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C251" t="s">
         <v>405</v>
@@ -6088,7 +6088,7 @@
         <v>19</v>
       </c>
       <c r="B252">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C252" t="s">
         <v>407</v>
@@ -6102,7 +6102,7 @@
         <v>19</v>
       </c>
       <c r="B253">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C253" t="s">
         <v>409</v>
@@ -6116,7 +6116,7 @@
         <v>19</v>
       </c>
       <c r="B254">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C254" t="s">
         <v>410</v>
@@ -6130,7 +6130,7 @@
         <v>19</v>
       </c>
       <c r="B255">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C255" t="s">
         <v>411</v>
@@ -6144,7 +6144,7 @@
         <v>19</v>
       </c>
       <c r="B256">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C256" t="s">
         <v>412</v>
@@ -6158,7 +6158,7 @@
         <v>19</v>
       </c>
       <c r="B257">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C257" t="s">
         <v>414</v>

</xml_diff>

<commit_message>
Add more medium level stores
</commit_message>
<xml_diff>
--- a/moreWorkingData.xlsx
+++ b/moreWorkingData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Navi\Documents\School\CS 438 (Big Data)\LetsGetThisBread\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5424BD-7C71-48B8-B7DA-A7BFE204EE57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9BD740-6916-45B9-9358-EF6A5CD27EE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25598" windowHeight="15998" xr2:uid="{224DDC23-A165-FE48-9542-0EB173C9A9C5}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="492">
   <si>
     <t>Grocery Store Name</t>
   </si>
@@ -1347,6 +1347,165 @@
   </si>
   <si>
     <t>"98042"</t>
+  </si>
+  <si>
+    <t>9620 28th Ave SW, Seattle, WA 98126</t>
+  </si>
+  <si>
+    <t>3900 S Othello St, Seattle, WA 98118</t>
+  </si>
+  <si>
+    <t>"98118"</t>
+  </si>
+  <si>
+    <t>210 Washington Ave S, Kent, WA 98032</t>
+  </si>
+  <si>
+    <t>7340 35th Ave NE, Seattle, WA 98115</t>
+  </si>
+  <si>
+    <t>26916 Maple Valley Hwy, Maple Valley, WA 98038</t>
+  </si>
+  <si>
+    <t>9262 Rainier Ave S, Seattle, WA 98118</t>
+  </si>
+  <si>
+    <t>2622 California Ave SW, Seattle, WA 98116</t>
+  </si>
+  <si>
+    <t>13101 SE Kent-Kangley Rd, Kent, WA 98030</t>
+  </si>
+  <si>
+    <t>17202 15th Ave NE, Shoreline, WA 98155</t>
+  </si>
+  <si>
+    <t>"98155"</t>
+  </si>
+  <si>
+    <t>27035 Pacific Hwy S, Des Moines, WA 98198</t>
+  </si>
+  <si>
+    <t>"98198"</t>
+  </si>
+  <si>
+    <t>2109 SW 336th St, Federal Way, WA 98023</t>
+  </si>
+  <si>
+    <t>6911 Coal Creek Pkwy SE, Newcastle, WA 98059</t>
+  </si>
+  <si>
+    <t>"98059"</t>
+  </si>
+  <si>
+    <t>17023 SE 272nd St, Covington, WA 98042</t>
+  </si>
+  <si>
+    <t>1645 140th Ave NE, Bellevue, WA 98005</t>
+  </si>
+  <si>
+    <t>"98005"</t>
+  </si>
+  <si>
+    <t>630 228th Ave NE, Sammamish, WA 98074</t>
+  </si>
+  <si>
+    <t>15100 SE 38th St, Bellevue, WA 98006</t>
+  </si>
+  <si>
+    <t>735 NW Gilman Blvd, Issaquah, WA 98027</t>
+  </si>
+  <si>
+    <t>6850 NE Bothell Way, Kenmore, WA 98028</t>
+  </si>
+  <si>
+    <t>19150 NE Woodinville Duvall Rd, Woodinville, WA 98077</t>
+  </si>
+  <si>
+    <t>"98077"</t>
+  </si>
+  <si>
+    <t>12519 NE 85th St, Kirkland, WA 98033</t>
+  </si>
+  <si>
+    <t>17230 140th Ave SE, Renton, WA 98058</t>
+  </si>
+  <si>
+    <t>"98058"</t>
+  </si>
+  <si>
+    <t>200 S 3rd St, Renton, WA 98057</t>
+  </si>
+  <si>
+    <t>4300 NE 4th St, Renton, WA 98059</t>
+  </si>
+  <si>
+    <t>3707 N Main St, Vancouver, WA 98663</t>
+  </si>
+  <si>
+    <t>"98663"</t>
+  </si>
+  <si>
+    <t>6701 E Mill Plain Blvd, Vancouver, WA 98661</t>
+  </si>
+  <si>
+    <t>408 NE 81st St, Vancouver, WA 98665</t>
+  </si>
+  <si>
+    <t>6711 NE 63rd St, Vancouver, WA 98661</t>
+  </si>
+  <si>
+    <t>6194 SW Murray Blvd, Beaverton, OR 97008</t>
+  </si>
+  <si>
+    <t>2177 NW 185th Ave, Hillsboro, OR 97124</t>
+  </si>
+  <si>
+    <t>2525 SE Tualatin Valley Hwy, Hillsboro, OR 97123</t>
+  </si>
+  <si>
+    <t>14555 SW Teal Blvd, Beaverton, OR 97007</t>
+  </si>
+  <si>
+    <t>15570 SW Pacific Hwy, Tigard, OR 97224</t>
+  </si>
+  <si>
+    <t>2836 Pacific Ave, Forest Grove, OR 97116</t>
+  </si>
+  <si>
+    <t>"97116"</t>
+  </si>
+  <si>
+    <t>4320 SE King Rd, Milwaukie, OR 97222</t>
+  </si>
+  <si>
+    <t>"97222"</t>
+  </si>
+  <si>
+    <t>401 A Ave, Lake Oswego, OR 97034</t>
+  </si>
+  <si>
+    <t>20685 SW Roy Rogers Rd, Sherwood, OR 97140</t>
+  </si>
+  <si>
+    <t>17779 SW Ferry Rd, Lake Oswego, OR 97035</t>
+  </si>
+  <si>
+    <t>95 82nd Dr, Gladstone, OR 97027</t>
+  </si>
+  <si>
+    <t>"97027"</t>
+  </si>
+  <si>
+    <t>13434 Colton Pl, Oregon City, OR 97045</t>
+  </si>
+  <si>
+    <t>14840 SE Webster Rd, Milwaukie, OR 97267</t>
+  </si>
+  <si>
+    <t>20151 SE Hwy 212, Boring, OR 97089</t>
+  </si>
+  <si>
+    <t>"97089"</t>
   </si>
 </sst>
 </file>
@@ -1720,10 +1879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9739F2B-2F3B-DD45-BA29-3AA82495FC82}">
-  <dimension ref="A1:H274"/>
+  <dimension ref="A1:I315"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B256" zoomScale="75" workbookViewId="0">
-      <selection activeCell="B276" sqref="B276"/>
+    <sheetView tabSelected="1" topLeftCell="B291" zoomScale="75" workbookViewId="0">
+      <selection activeCell="D315" sqref="D315"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1737,7 +1896,7 @@
     <col min="7" max="7" width="22" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1760,7 +1919,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1782,8 +1941,12 @@
       <c r="G2" s="1">
         <v>23200</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="I2">
+        <f>COUNTIF(B2:B300,"1")</f>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1805,8 +1968,12 @@
       <c r="G3" s="1">
         <v>29007</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="I3">
+        <f>COUNTIF(B2:B301,"2")</f>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1828,8 +1995,12 @@
       <c r="G4" s="1">
         <v>22668</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="I4">
+        <f>COUNTIF(B2:B302,"3")</f>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1852,7 +2023,7 @@
         <v>8395</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1875,7 +2046,7 @@
         <v>27612</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1898,7 +2069,7 @@
         <v>30072</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1921,7 +2092,7 @@
         <v>9915</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1944,7 +2115,7 @@
         <v>23200</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1967,7 +2138,7 @@
         <v>30688</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1990,7 +2161,7 @@
         <v>10676</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2013,7 +2184,7 @@
         <v>22668</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -2036,7 +2207,7 @@
         <v>37097</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -2059,7 +2230,7 @@
         <v>45454</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -2082,7 +2253,7 @@
         <v>37097</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -6472,6 +6643,580 @@
       </c>
       <c r="D274" t="s">
         <v>438</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A275" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B275">
+        <v>2</v>
+      </c>
+      <c r="C275" t="s">
+        <v>439</v>
+      </c>
+      <c r="D275" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A276" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B276">
+        <v>2</v>
+      </c>
+      <c r="C276" t="s">
+        <v>440</v>
+      </c>
+      <c r="D276" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A277" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B277">
+        <v>2</v>
+      </c>
+      <c r="C277" t="s">
+        <v>442</v>
+      </c>
+      <c r="D277" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A278" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B278">
+        <v>2</v>
+      </c>
+      <c r="C278" t="s">
+        <v>443</v>
+      </c>
+      <c r="D278" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A279" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B279">
+        <v>2</v>
+      </c>
+      <c r="C279" t="s">
+        <v>444</v>
+      </c>
+      <c r="D279" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A280" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B280">
+        <v>2</v>
+      </c>
+      <c r="C280" t="s">
+        <v>445</v>
+      </c>
+      <c r="D280" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A281" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B281">
+        <v>2</v>
+      </c>
+      <c r="C281" t="s">
+        <v>446</v>
+      </c>
+      <c r="D281" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A282" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B282">
+        <v>2</v>
+      </c>
+      <c r="C282" t="s">
+        <v>447</v>
+      </c>
+      <c r="D282" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A283" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B283">
+        <v>2</v>
+      </c>
+      <c r="C283" t="s">
+        <v>448</v>
+      </c>
+      <c r="D283" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A284" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B284">
+        <v>2</v>
+      </c>
+      <c r="C284" t="s">
+        <v>450</v>
+      </c>
+      <c r="D284" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A285" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B285">
+        <v>2</v>
+      </c>
+      <c r="C285" t="s">
+        <v>452</v>
+      </c>
+      <c r="D285" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A286" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B286">
+        <v>2</v>
+      </c>
+      <c r="C286" t="s">
+        <v>453</v>
+      </c>
+      <c r="D286" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A287" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B287">
+        <v>2</v>
+      </c>
+      <c r="C287" t="s">
+        <v>455</v>
+      </c>
+      <c r="D287" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A288" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B288">
+        <v>2</v>
+      </c>
+      <c r="C288" t="s">
+        <v>456</v>
+      </c>
+      <c r="D288" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A289" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B289">
+        <v>2</v>
+      </c>
+      <c r="C289" t="s">
+        <v>458</v>
+      </c>
+      <c r="D289" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A290" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B290">
+        <v>2</v>
+      </c>
+      <c r="C290" t="s">
+        <v>459</v>
+      </c>
+      <c r="D290" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A291" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B291">
+        <v>2</v>
+      </c>
+      <c r="C291" t="s">
+        <v>460</v>
+      </c>
+      <c r="D291" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A292" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B292">
+        <v>2</v>
+      </c>
+      <c r="C292" t="s">
+        <v>461</v>
+      </c>
+      <c r="D292" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A293" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B293">
+        <v>2</v>
+      </c>
+      <c r="C293" t="s">
+        <v>462</v>
+      </c>
+      <c r="D293" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A294" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B294">
+        <v>2</v>
+      </c>
+      <c r="C294" t="s">
+        <v>464</v>
+      </c>
+      <c r="D294" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A295" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B295">
+        <v>2</v>
+      </c>
+      <c r="C295" t="s">
+        <v>465</v>
+      </c>
+      <c r="D295" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A296" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B296">
+        <v>2</v>
+      </c>
+      <c r="C296" t="s">
+        <v>467</v>
+      </c>
+      <c r="D296" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A297" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B297">
+        <v>2</v>
+      </c>
+      <c r="C297" t="s">
+        <v>468</v>
+      </c>
+      <c r="D297" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A298" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B298">
+        <v>2</v>
+      </c>
+      <c r="C298" t="s">
+        <v>469</v>
+      </c>
+      <c r="D298" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A299" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B299">
+        <v>2</v>
+      </c>
+      <c r="C299" t="s">
+        <v>471</v>
+      </c>
+      <c r="D299" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A300" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B300">
+        <v>2</v>
+      </c>
+      <c r="C300" t="s">
+        <v>472</v>
+      </c>
+      <c r="D300" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A301" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B301">
+        <v>2</v>
+      </c>
+      <c r="C301" t="s">
+        <v>473</v>
+      </c>
+      <c r="D301" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A302" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B302">
+        <v>2</v>
+      </c>
+      <c r="C302" t="s">
+        <v>474</v>
+      </c>
+      <c r="D302" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A303" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B303">
+        <v>2</v>
+      </c>
+      <c r="C303" t="s">
+        <v>475</v>
+      </c>
+      <c r="D303" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A304" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B304">
+        <v>2</v>
+      </c>
+      <c r="C304" t="s">
+        <v>476</v>
+      </c>
+      <c r="D304" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A305" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B305">
+        <v>2</v>
+      </c>
+      <c r="C305" t="s">
+        <v>477</v>
+      </c>
+      <c r="D305" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A306" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B306">
+        <v>2</v>
+      </c>
+      <c r="C306" t="s">
+        <v>478</v>
+      </c>
+      <c r="D306" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A307" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B307">
+        <v>2</v>
+      </c>
+      <c r="C307" t="s">
+        <v>479</v>
+      </c>
+      <c r="D307" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A308" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B308">
+        <v>2</v>
+      </c>
+      <c r="C308" t="s">
+        <v>481</v>
+      </c>
+      <c r="D308" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A309" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B309">
+        <v>2</v>
+      </c>
+      <c r="C309" t="s">
+        <v>483</v>
+      </c>
+      <c r="D309" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A310" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B310">
+        <v>2</v>
+      </c>
+      <c r="C310" t="s">
+        <v>484</v>
+      </c>
+      <c r="D310" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A311" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B311">
+        <v>2</v>
+      </c>
+      <c r="C311" t="s">
+        <v>485</v>
+      </c>
+      <c r="D311" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A312" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B312">
+        <v>2</v>
+      </c>
+      <c r="C312" t="s">
+        <v>486</v>
+      </c>
+      <c r="D312" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A313" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B313">
+        <v>2</v>
+      </c>
+      <c r="C313" t="s">
+        <v>488</v>
+      </c>
+      <c r="D313" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A314" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B314">
+        <v>2</v>
+      </c>
+      <c r="C314" t="s">
+        <v>489</v>
+      </c>
+      <c r="D314" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A315" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B315">
+        <v>2</v>
+      </c>
+      <c r="C315" t="s">
+        <v>490</v>
+      </c>
+      <c r="D315" t="s">
+        <v>491</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added some population and income data to stuff that Navreen added
</commit_message>
<xml_diff>
--- a/moreWorkingData.xlsx
+++ b/moreWorkingData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Navi\Documents\School\CS 438 (Big Data)\LetsGetThisBread\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mitchell.nguyen/school/senior year/spring 2019/big data/zzz letsGetThisBread/github/LetsGetThisBread/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9BD740-6916-45B9-9358-EF6A5CD27EE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2E942A-9ABD-1D41-B147-FD056D583C84}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25598" windowHeight="15998" xr2:uid="{224DDC23-A165-FE48-9542-0EB173C9A9C5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{224DDC23-A165-FE48-9542-0EB173C9A9C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1555,7 +1556,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1565,6 +1566,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1881,22 +1884,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9739F2B-2F3B-DD45-BA29-3AA82495FC82}">
   <dimension ref="A1:I315"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B291" zoomScale="75" workbookViewId="0">
-      <selection activeCell="D315" sqref="D315"/>
+    <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
+      <selection activeCell="E246" sqref="E246"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.8125" customWidth="1"/>
-    <col min="2" max="2" width="12.3125" customWidth="1"/>
-    <col min="3" max="3" width="69.6875" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="69.6640625" customWidth="1"/>
     <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="25.6875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="27.1875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.1640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="22" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1919,7 +1922,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1946,7 +1949,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1973,7 +1976,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2000,7 +2003,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2023,7 +2026,7 @@
         <v>8395</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -2046,7 +2049,7 @@
         <v>27612</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -2069,7 +2072,7 @@
         <v>30072</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2092,7 +2095,7 @@
         <v>9915</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2115,7 +2118,7 @@
         <v>23200</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2138,7 +2141,7 @@
         <v>30688</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2161,7 +2164,7 @@
         <v>10676</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2184,7 +2187,7 @@
         <v>22668</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -2207,7 +2210,7 @@
         <v>37097</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -2230,7 +2233,7 @@
         <v>45454</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -2253,7 +2256,7 @@
         <v>37097</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -2276,7 +2279,7 @@
         <v>30072</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -2299,7 +2302,7 @@
         <v>28254</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -2322,7 +2325,7 @@
         <v>17978</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -2345,7 +2348,7 @@
         <v>27612</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -2368,7 +2371,7 @@
         <v>29007</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -2391,7 +2394,7 @@
         <v>45454</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -2414,7 +2417,7 @@
         <v>28254</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -2437,7 +2440,7 @@
         <v>27422</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -2460,7 +2463,7 @@
         <v>31968</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -2483,7 +2486,7 @@
         <v>30072</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -2506,7 +2509,7 @@
         <v>12340</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -2529,7 +2532,7 @@
         <v>10676</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -2552,7 +2555,7 @@
         <v>27612</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -2575,7 +2578,7 @@
         <v>30072</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -2598,7 +2601,7 @@
         <v>8395</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -2621,7 +2624,7 @@
         <v>10676</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -2644,7 +2647,7 @@
         <v>37062</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -2667,7 +2670,7 @@
         <v>22668</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -2690,7 +2693,7 @@
         <v>29007</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -2713,7 +2716,7 @@
         <v>27422</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -2736,7 +2739,7 @@
         <v>27705</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -2759,7 +2762,7 @@
         <v>17978</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>45</v>
       </c>
@@ -2782,7 +2785,7 @@
         <v>27612</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -2805,7 +2808,7 @@
         <v>30688</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -2828,7 +2831,7 @@
         <v>29007</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -2851,7 +2854,7 @@
         <v>10676</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -2874,7 +2877,7 @@
         <v>8395</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -2897,7 +2900,7 @@
         <v>12340</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -2920,7 +2923,7 @@
         <v>22668</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -2943,7 +2946,7 @@
         <v>37097</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -2966,7 +2969,7 @@
         <v>45454</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -2989,7 +2992,7 @@
         <v>37062</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -3012,7 +3015,7 @@
         <v>27705</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>45</v>
       </c>
@@ -3035,7 +3038,7 @@
         <v>33590</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>45</v>
       </c>
@@ -3058,7 +3061,7 @@
         <v>31968</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>45</v>
       </c>
@@ -3081,7 +3084,7 @@
         <v>17978</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>60</v>
       </c>
@@ -3104,7 +3107,7 @@
         <v>30072</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>60</v>
       </c>
@@ -3127,7 +3130,7 @@
         <v>6682</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>60</v>
       </c>
@@ -3150,7 +3153,7 @@
         <v>27422</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -3173,7 +3176,7 @@
         <v>37097</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -3196,7 +3199,7 @@
         <v>13563</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>60</v>
       </c>
@@ -3219,7 +3222,7 @@
         <v>8721</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>4</v>
       </c>
@@ -3243,7 +3246,7 @@
       </c>
       <c r="H58" s="6"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>4</v>
       </c>
@@ -3266,7 +3269,7 @@
         <v>44673</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>4</v>
       </c>
@@ -3289,7 +3292,7 @@
         <v>37105</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>4</v>
       </c>
@@ -3312,7 +3315,7 @@
         <v>58442</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>4</v>
       </c>
@@ -3335,7 +3338,7 @@
         <v>40407</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>4</v>
       </c>
@@ -3358,7 +3361,7 @@
         <v>27946</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>4</v>
       </c>
@@ -3381,7 +3384,7 @@
         <v>36000</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>4</v>
       </c>
@@ -3404,7 +3407,7 @@
         <v>46206</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>4</v>
       </c>
@@ -3427,7 +3430,7 @@
         <v>21077</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>4</v>
       </c>
@@ -3450,7 +3453,7 @@
         <v>12628</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
         <v>4</v>
       </c>
@@ -3473,7 +3476,7 @@
         <v>21039</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
         <v>4</v>
       </c>
@@ -3496,7 +3499,7 @@
         <v>26944</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>4</v>
       </c>
@@ -3519,7 +3522,7 @@
         <v>30321</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
         <v>4</v>
       </c>
@@ -3542,7 +3545,7 @@
         <v>30832</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>9</v>
       </c>
@@ -3565,7 +3568,7 @@
         <v>21147</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
         <v>9</v>
       </c>
@@ -3588,7 +3591,7 @@
         <v>23741</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>9</v>
       </c>
@@ -3611,7 +3614,7 @@
         <v>30832</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>9</v>
       </c>
@@ -3634,7 +3637,7 @@
         <v>17089</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
         <v>9</v>
       </c>
@@ -3657,7 +3660,7 @@
         <v>23586</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
         <v>9</v>
       </c>
@@ -3680,7 +3683,7 @@
         <v>24189</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>9</v>
       </c>
@@ -3703,7 +3706,7 @@
         <v>38290</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
         <v>9</v>
       </c>
@@ -3726,7 +3729,7 @@
         <v>56025</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
         <v>9</v>
       </c>
@@ -3749,7 +3752,7 @@
         <v>21781</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
         <v>9</v>
       </c>
@@ -3772,7 +3775,7 @@
         <v>22699</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
         <v>23</v>
       </c>
@@ -3795,7 +3798,7 @@
         <v>27763</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
         <v>23</v>
       </c>
@@ -3818,7 +3821,7 @@
         <v>27899</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
         <v>23</v>
       </c>
@@ -3841,7 +3844,7 @@
         <v>31968</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>23</v>
       </c>
@@ -3864,7 +3867,7 @@
         <v>17171</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
         <v>23</v>
       </c>
@@ -3887,7 +3890,7 @@
         <v>26217</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
         <v>23</v>
       </c>
@@ -3910,7 +3913,7 @@
         <v>26168</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
         <v>23</v>
       </c>
@@ -3933,7 +3936,7 @@
         <v>28896</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
         <v>23</v>
       </c>
@@ -3956,7 +3959,7 @@
         <v>24170</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
         <v>23</v>
       </c>
@@ -3979,7 +3982,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
         <v>23</v>
       </c>
@@ -4002,7 +4005,7 @@
         <v>9703</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
         <v>23</v>
       </c>
@@ -4025,7 +4028,7 @@
         <v>50792</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
         <v>23</v>
       </c>
@@ -4048,7 +4051,7 @@
         <v>41740</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
         <v>23</v>
       </c>
@@ -4071,7 +4074,7 @@
         <v>11948</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
         <v>23</v>
       </c>
@@ -4094,7 +4097,7 @@
         <v>44555</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
         <v>23</v>
       </c>
@@ -4117,7 +4120,7 @@
         <v>34338</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
         <v>23</v>
       </c>
@@ -4140,7 +4143,7 @@
         <v>24411</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
         <v>23</v>
       </c>
@@ -4163,7 +4166,7 @@
         <v>31365</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
         <v>23</v>
       </c>
@@ -4186,7 +4189,7 @@
         <v>32086</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
         <v>23</v>
       </c>
@@ -4209,7 +4212,7 @@
         <v>44151</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="4" t="s">
         <v>23</v>
       </c>
@@ -4222,8 +4225,17 @@
       <c r="D101" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="E101" s="7">
+        <v>73266.001499999998</v>
+      </c>
+      <c r="F101" s="7">
+        <v>81097.512499999997</v>
+      </c>
+      <c r="G101" s="7">
+        <v>51802</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
         <v>23</v>
       </c>
@@ -4236,8 +4248,17 @@
       <c r="D102" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="E102" s="8">
+        <v>60383</v>
+      </c>
+      <c r="F102" s="8">
+        <v>69930</v>
+      </c>
+      <c r="G102" s="8">
+        <v>34354</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="4" t="s">
         <v>23</v>
       </c>
@@ -4250,8 +4271,17 @@
       <c r="D103" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="E103" s="7">
+        <v>86310.062399999995</v>
+      </c>
+      <c r="F103" s="7">
+        <v>100545.59880000001</v>
+      </c>
+      <c r="G103" s="7">
+        <v>20419</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
         <v>23</v>
       </c>
@@ -4264,8 +4294,17 @@
       <c r="D104" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="E104" s="7">
+        <v>65442.285100000001</v>
+      </c>
+      <c r="F104" s="7">
+        <v>77874.890400000004</v>
+      </c>
+      <c r="G104" s="7">
+        <v>36581</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" s="4" t="s">
         <v>23</v>
       </c>
@@ -4278,8 +4317,17 @@
       <c r="D105" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="E105" s="7">
+        <v>72611.400099999999</v>
+      </c>
+      <c r="F105" s="7">
+        <v>84069.011799999993</v>
+      </c>
+      <c r="G105" s="7">
+        <v>20166</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
         <v>23</v>
       </c>
@@ -4292,8 +4340,17 @@
       <c r="D106" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="E106" s="7">
+        <v>47909.716200000003</v>
+      </c>
+      <c r="F106" s="7">
+        <v>60487.025099999999</v>
+      </c>
+      <c r="G106" s="7">
+        <v>30826</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" s="4" t="s">
         <v>23</v>
       </c>
@@ -4306,8 +4363,17 @@
       <c r="D107" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="E107" s="7">
+        <v>65884.25</v>
+      </c>
+      <c r="F107" s="7">
+        <v>74377.8217</v>
+      </c>
+      <c r="G107" s="7">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" s="4" t="s">
         <v>23</v>
       </c>
@@ -4320,8 +4386,17 @@
       <c r="D108" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="E108" s="7">
+        <v>37928.792000000001</v>
+      </c>
+      <c r="F108" s="7">
+        <v>53564.7883</v>
+      </c>
+      <c r="G108" s="7">
+        <v>29750</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" s="4" t="s">
         <v>23</v>
       </c>
@@ -4334,8 +4409,17 @@
       <c r="D109" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="E109" s="8">
+        <v>57971</v>
+      </c>
+      <c r="F109" s="8">
+        <v>77731</v>
+      </c>
+      <c r="G109" s="8">
+        <v>31454</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" s="4" t="s">
         <v>23</v>
       </c>
@@ -4348,8 +4432,17 @@
       <c r="D110" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="E110" s="7">
+        <v>58102.518799999998</v>
+      </c>
+      <c r="F110" s="7">
+        <v>69258.310599999997</v>
+      </c>
+      <c r="G110" s="7">
+        <v>21610</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
         <v>23</v>
       </c>
@@ -4362,8 +4455,17 @@
       <c r="D111" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="E111" s="7">
+        <v>58029.2039</v>
+      </c>
+      <c r="F111" s="7">
+        <v>75946.443799999994</v>
+      </c>
+      <c r="G111" s="7">
+        <v>30491</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" s="4" t="s">
         <v>23</v>
       </c>
@@ -4376,8 +4478,17 @@
       <c r="D112" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E112" s="7">
+        <v>64104.886400000003</v>
+      </c>
+      <c r="F112" s="7">
+        <v>76263.776299999998</v>
+      </c>
+      <c r="G112" s="7">
+        <v>32489</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" s="4" t="s">
         <v>23</v>
       </c>
@@ -4390,8 +4501,17 @@
       <c r="D113" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E113" s="7">
+        <v>43856.498299999999</v>
+      </c>
+      <c r="F113" s="7">
+        <v>48426.440900000001</v>
+      </c>
+      <c r="G113" s="7">
+        <v>22989</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" s="4" t="s">
         <v>23</v>
       </c>
@@ -4404,8 +4524,17 @@
       <c r="D114" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E114" s="7">
+        <v>55776.7857</v>
+      </c>
+      <c r="F114" s="7">
+        <v>65497.991600000001</v>
+      </c>
+      <c r="G114" s="7">
+        <v>24092</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" s="4" t="s">
         <v>23</v>
       </c>
@@ -4418,8 +4547,17 @@
       <c r="D115" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E115" s="7">
+        <v>54158</v>
+      </c>
+      <c r="F115" s="7">
+        <v>74219</v>
+      </c>
+      <c r="G115" s="7">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" s="4" t="s">
         <v>23</v>
       </c>
@@ -4432,8 +4570,17 @@
       <c r="D116" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E116" s="7">
+        <v>51833.886500000001</v>
+      </c>
+      <c r="F116" s="7">
+        <v>64255.244200000001</v>
+      </c>
+      <c r="G116" s="7">
+        <v>33853</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" s="4" t="s">
         <v>23</v>
       </c>
@@ -4446,8 +4593,17 @@
       <c r="D117" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E117" s="7">
+        <v>65193.957900000001</v>
+      </c>
+      <c r="F117" s="7">
+        <v>75131.595100000006</v>
+      </c>
+      <c r="G117" s="7">
+        <v>40815</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" s="4" t="s">
         <v>23</v>
       </c>
@@ -4460,8 +4616,17 @@
       <c r="D118" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E118" s="7">
+        <v>40585.642800000001</v>
+      </c>
+      <c r="F118" s="7">
+        <v>49092.392599999999</v>
+      </c>
+      <c r="G118" s="7">
+        <v>31647</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" s="4" t="s">
         <v>213</v>
       </c>
@@ -4474,8 +4639,17 @@
       <c r="D119" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E119" s="7">
+        <v>58304.0193</v>
+      </c>
+      <c r="F119" s="7">
+        <v>70671.428700000004</v>
+      </c>
+      <c r="G119" s="7">
+        <v>30832</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" s="4" t="s">
         <v>213</v>
       </c>
@@ -4488,8 +4662,17 @@
       <c r="D120" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E120" s="7">
+        <v>55155.441299999999</v>
+      </c>
+      <c r="F120" s="7">
+        <v>77891.291200000007</v>
+      </c>
+      <c r="G120" s="7">
+        <v>10676</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" s="4" t="s">
         <v>213</v>
       </c>
@@ -4502,8 +4685,17 @@
       <c r="D121" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E121" s="7">
+        <v>61295.774100000002</v>
+      </c>
+      <c r="F121" s="7">
+        <v>90869.362200000003</v>
+      </c>
+      <c r="G121" s="7">
+        <v>9915</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" s="4" t="s">
         <v>213</v>
       </c>
@@ -4516,8 +4708,17 @@
       <c r="D122" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E122" s="7">
+        <v>52559.811500000003</v>
+      </c>
+      <c r="F122" s="7">
+        <v>66785.020699999994</v>
+      </c>
+      <c r="G122" s="7">
+        <v>37097</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" s="4" t="s">
         <v>213</v>
       </c>
@@ -4530,8 +4731,17 @@
       <c r="D123" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E123" s="7">
+        <v>76045.592099999994</v>
+      </c>
+      <c r="F123" s="7">
+        <v>93289.298999999999</v>
+      </c>
+      <c r="G123" s="7">
+        <v>17089</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" s="4" t="s">
         <v>213</v>
       </c>
@@ -4544,8 +4754,17 @@
       <c r="D124" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E124" s="7">
+        <v>45265.474999999999</v>
+      </c>
+      <c r="F124" s="7">
+        <v>56202.1921</v>
+      </c>
+      <c r="G124" s="7">
+        <v>23741</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" s="4" t="s">
         <v>213</v>
       </c>
@@ -4558,8 +4777,17 @@
       <c r="D125" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E125" s="7">
+        <v>63322.856099999997</v>
+      </c>
+      <c r="F125" s="7">
+        <v>75211.098899999997</v>
+      </c>
+      <c r="G125" s="7">
+        <v>38290</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" s="4" t="s">
         <v>213</v>
       </c>
@@ -4572,8 +4800,17 @@
       <c r="D126" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E126" s="7">
+        <v>71692.024600000004</v>
+      </c>
+      <c r="F126" s="7">
+        <v>96371.055800000002</v>
+      </c>
+      <c r="G126" s="7">
+        <v>23586</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" s="4" t="s">
         <v>213</v>
       </c>
@@ -4586,8 +4823,17 @@
       <c r="D127" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E127" s="7">
+        <v>50941.976699999999</v>
+      </c>
+      <c r="F127" s="7">
+        <v>63876.736299999997</v>
+      </c>
+      <c r="G127" s="7">
+        <v>36792</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" s="4" t="s">
         <v>213</v>
       </c>
@@ -4600,8 +4846,17 @@
       <c r="D128" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E128" s="7">
+        <v>46533.762900000002</v>
+      </c>
+      <c r="F128" s="7">
+        <v>60501.269699999997</v>
+      </c>
+      <c r="G128" s="7">
+        <v>40602</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" s="4" t="s">
         <v>213</v>
       </c>
@@ -4614,8 +4869,17 @@
       <c r="D129" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E129" s="7">
+        <v>58029.2039</v>
+      </c>
+      <c r="F129" s="7">
+        <v>75946.443799999994</v>
+      </c>
+      <c r="G129" s="7">
+        <v>30491</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" s="4" t="s">
         <v>213</v>
       </c>
@@ -4628,8 +4892,17 @@
       <c r="D130" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E130" s="7">
+        <v>55555.897400000002</v>
+      </c>
+      <c r="F130" s="7">
+        <v>69343.763099999996</v>
+      </c>
+      <c r="G130" s="7">
+        <v>26944</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" s="4" t="s">
         <v>213</v>
       </c>
@@ -4642,8 +4915,17 @@
       <c r="D131" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E131" s="7">
+        <v>35363.476199999997</v>
+      </c>
+      <c r="F131" s="7">
+        <v>51785.846700000002</v>
+      </c>
+      <c r="G131" s="7">
+        <v>37105</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" s="4" t="s">
         <v>213</v>
       </c>
@@ -4656,8 +4938,17 @@
       <c r="D132" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E132" s="7">
+        <v>52409.904600000002</v>
+      </c>
+      <c r="F132" s="7">
+        <v>63083.267999999996</v>
+      </c>
+      <c r="G132" s="7">
+        <v>44151</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" s="4" t="s">
         <v>213</v>
       </c>
@@ -4670,8 +4961,17 @@
       <c r="D133" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E133" s="7">
+        <v>56657.259400000003</v>
+      </c>
+      <c r="F133" s="7">
+        <v>68952.066699999996</v>
+      </c>
+      <c r="G133" s="7">
+        <v>33769</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" s="4" t="s">
         <v>213</v>
       </c>
@@ -4684,8 +4984,17 @@
       <c r="D134" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E134" s="7">
+        <v>58076.582799999996</v>
+      </c>
+      <c r="F134" s="7">
+        <v>73848.590299999996</v>
+      </c>
+      <c r="G134" s="7">
+        <v>44673</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" s="4" t="s">
         <v>213</v>
       </c>
@@ -4698,8 +5007,17 @@
       <c r="D135" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E135" s="7">
+        <v>50182.7209</v>
+      </c>
+      <c r="F135" s="7">
+        <v>63245.567300000002</v>
+      </c>
+      <c r="G135" s="7">
+        <v>10010</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" s="4" t="s">
         <v>213</v>
       </c>
@@ -4712,8 +5030,17 @@
       <c r="D136" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E136" s="7">
+        <v>75727.902199999997</v>
+      </c>
+      <c r="F136" s="7">
+        <v>101536.89659999999</v>
+      </c>
+      <c r="G136" s="7">
+        <v>22241</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" s="4" t="s">
         <v>213</v>
       </c>
@@ -4726,8 +5053,17 @@
       <c r="D137" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E137" s="7">
+        <v>94297.2359</v>
+      </c>
+      <c r="F137" s="7">
+        <v>119650.6066</v>
+      </c>
+      <c r="G137" s="7">
+        <v>26141</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" s="4" t="s">
         <v>213</v>
       </c>
@@ -4740,8 +5076,17 @@
       <c r="D138" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E138" s="7">
+        <v>57970.935599999997</v>
+      </c>
+      <c r="F138" s="7">
+        <v>77731.271099999998</v>
+      </c>
+      <c r="G138" s="7">
+        <v>31454</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" s="4" t="s">
         <v>213</v>
       </c>
@@ -4754,8 +5099,17 @@
       <c r="D139" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E139" s="7">
+        <v>99669.231299999999</v>
+      </c>
+      <c r="F139" s="7">
+        <v>144247.85560000001</v>
+      </c>
+      <c r="G139" s="7">
+        <v>27946</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" s="4" t="s">
         <v>213</v>
       </c>
@@ -4768,8 +5122,17 @@
       <c r="D140" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E140" s="7">
+        <v>61978.389199999998</v>
+      </c>
+      <c r="F140" s="7">
+        <v>85612.291899999997</v>
+      </c>
+      <c r="G140" s="7">
+        <v>20715</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141" s="4" t="s">
         <v>213</v>
       </c>
@@ -4782,8 +5145,17 @@
       <c r="D141" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E141" s="7">
+        <v>134158.6286</v>
+      </c>
+      <c r="F141" s="7">
+        <v>157543.29089999999</v>
+      </c>
+      <c r="G141" s="7">
+        <v>25748</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" s="4" t="s">
         <v>213</v>
       </c>
@@ -4796,8 +5168,17 @@
       <c r="D142" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E142" s="7">
+        <v>69589.362099999998</v>
+      </c>
+      <c r="F142" s="7">
+        <v>84662.419800000003</v>
+      </c>
+      <c r="G142" s="7">
+        <v>24889</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" s="4" t="s">
         <v>213</v>
       </c>
@@ -4810,8 +5191,17 @@
       <c r="D143" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E143" s="7">
+        <v>66530.5717</v>
+      </c>
+      <c r="F143" s="7">
+        <v>80201.871799999994</v>
+      </c>
+      <c r="G143" s="7">
+        <v>19727</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" s="4" t="s">
         <v>213</v>
       </c>
@@ -4824,8 +5214,17 @@
       <c r="D144" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E144" s="7">
+        <v>64804.2264</v>
+      </c>
+      <c r="F144" s="7">
+        <v>79531.967600000004</v>
+      </c>
+      <c r="G144" s="7">
+        <v>21147</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145" s="4" t="s">
         <v>213</v>
       </c>
@@ -4838,8 +5237,17 @@
       <c r="D145" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E145" s="7">
+        <v>52145.068599999999</v>
+      </c>
+      <c r="F145" s="7">
+        <v>79895.078800000003</v>
+      </c>
+      <c r="G145" s="7">
+        <v>43924</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146" s="4" t="s">
         <v>213</v>
       </c>
@@ -4852,8 +5260,17 @@
       <c r="D146" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E146" s="7">
+        <v>93173.297000000006</v>
+      </c>
+      <c r="F146" s="7">
+        <v>111385.624</v>
+      </c>
+      <c r="G146" s="7">
+        <v>58442</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147" s="4" t="s">
         <v>213</v>
       </c>
@@ -4866,8 +5283,17 @@
       <c r="D147" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E147" s="7">
+        <v>78392.555999999997</v>
+      </c>
+      <c r="F147" s="7">
+        <v>93426.530100000004</v>
+      </c>
+      <c r="G147" s="7">
+        <v>40407</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148" s="4" t="s">
         <v>213</v>
       </c>
@@ -4880,8 +5306,17 @@
       <c r="D148" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E148" s="7">
+        <v>57182.2189</v>
+      </c>
+      <c r="F148" s="7">
+        <v>71395.290200000003</v>
+      </c>
+      <c r="G148" s="7">
+        <v>44555</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149" s="4" t="s">
         <v>254</v>
       </c>
@@ -4894,8 +5329,17 @@
       <c r="D149" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E149" s="7">
+        <v>52559.811500000003</v>
+      </c>
+      <c r="F149" s="7">
+        <v>66785.020699999994</v>
+      </c>
+      <c r="G149" s="7">
+        <v>37097</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" s="4" t="s">
         <v>254</v>
       </c>
@@ -4908,8 +5352,17 @@
       <c r="D150" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E150" s="7">
+        <v>56871.776400000002</v>
+      </c>
+      <c r="F150" s="7">
+        <v>70607.386499999993</v>
+      </c>
+      <c r="G150" s="7">
+        <v>16612</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" s="4" t="s">
         <v>254</v>
       </c>
@@ -4922,8 +5375,17 @@
       <c r="D151" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E151" s="7">
+        <v>68802.7641</v>
+      </c>
+      <c r="F151" s="7">
+        <v>94200.623399999997</v>
+      </c>
+      <c r="G151" s="7">
+        <v>21781</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152" s="4" t="s">
         <v>254</v>
       </c>
@@ -4936,8 +5398,17 @@
       <c r="D152" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E152" s="7">
+        <v>85739.599400000006</v>
+      </c>
+      <c r="F152" s="7">
+        <v>106388.55220000001</v>
+      </c>
+      <c r="G152" s="7">
+        <v>13888</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153" s="4" t="s">
         <v>254</v>
       </c>
@@ -4950,8 +5421,17 @@
       <c r="D153" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E153" s="7">
+        <v>99661.716199999995</v>
+      </c>
+      <c r="F153" s="7">
+        <v>115316.9586</v>
+      </c>
+      <c r="G153" s="7">
+        <v>24348</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154" s="4" t="s">
         <v>34</v>
       </c>
@@ -4964,8 +5444,17 @@
       <c r="D154" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E154" s="7">
+        <v>99661.716199999995</v>
+      </c>
+      <c r="F154" s="7">
+        <v>115316.9586</v>
+      </c>
+      <c r="G154" s="7">
+        <v>24348</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155" s="4" t="s">
         <v>254</v>
       </c>
@@ -4978,8 +5467,17 @@
       <c r="D155" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E155" s="7">
+        <v>94297.2359</v>
+      </c>
+      <c r="F155" s="7">
+        <v>119650.6066</v>
+      </c>
+      <c r="G155" s="7">
+        <v>26141</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156" s="4" t="s">
         <v>254</v>
       </c>
@@ -4992,8 +5490,17 @@
       <c r="D156" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E156" s="7">
+        <v>132143.89259999999</v>
+      </c>
+      <c r="F156" s="7">
+        <v>155991.59160000001</v>
+      </c>
+      <c r="G156" s="7">
+        <v>20715</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157" s="4" t="s">
         <v>254</v>
       </c>
@@ -5006,8 +5513,17 @@
       <c r="D157" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E157" s="7">
+        <v>94081.661399999997</v>
+      </c>
+      <c r="F157" s="7">
+        <v>104078.2985</v>
+      </c>
+      <c r="G157" s="7">
+        <v>31171</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A158" s="4" t="s">
         <v>34</v>
       </c>
@@ -5020,8 +5536,17 @@
       <c r="D158" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E158" s="7">
+        <v>94081.661399999997</v>
+      </c>
+      <c r="F158" s="7">
+        <v>104078.2985</v>
+      </c>
+      <c r="G158" s="7">
+        <v>31171</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159" s="4" t="s">
         <v>270</v>
       </c>
@@ -5034,8 +5559,17 @@
       <c r="D159" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E159" s="7">
+        <v>42244.986900000004</v>
+      </c>
+      <c r="F159" s="7">
+        <v>57949.0308</v>
+      </c>
+      <c r="G159" s="7">
+        <v>41740</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160" s="4" t="s">
         <v>270</v>
       </c>
@@ -5048,8 +5582,17 @@
       <c r="D160" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E160" s="7">
+        <v>48476.457799999996</v>
+      </c>
+      <c r="F160" s="7">
+        <v>55472.197800000002</v>
+      </c>
+      <c r="G160" s="7">
+        <v>45454</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161" s="4" t="s">
         <v>270</v>
       </c>
@@ -5062,8 +5605,17 @@
       <c r="D161" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E161" s="7">
+        <v>43212.265700000004</v>
+      </c>
+      <c r="F161" s="7">
+        <v>53688.117100000003</v>
+      </c>
+      <c r="G161" s="7">
+        <v>27422</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162" s="4" t="s">
         <v>270</v>
       </c>
@@ -5076,8 +5628,17 @@
       <c r="D162" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E162" s="7">
+        <v>45265.474999999999</v>
+      </c>
+      <c r="F162" s="7">
+        <v>56202.1921</v>
+      </c>
+      <c r="G162" s="7">
+        <v>23741</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" s="4" t="s">
         <v>270</v>
       </c>
@@ -5090,8 +5651,17 @@
       <c r="D163" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E163" s="7">
+        <v>66009.695600000006</v>
+      </c>
+      <c r="F163" s="7">
+        <v>80265.121199999994</v>
+      </c>
+      <c r="G163" s="7">
+        <v>42891</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" s="4" t="s">
         <v>270</v>
       </c>
@@ -5104,8 +5674,17 @@
       <c r="D164" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E164" s="7">
+        <v>76045.592099999994</v>
+      </c>
+      <c r="F164" s="7">
+        <v>93289.298999999999</v>
+      </c>
+      <c r="G164" s="7">
+        <v>17089</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" s="4" t="s">
         <v>270</v>
       </c>
@@ -5118,8 +5697,17 @@
       <c r="D165" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E165" s="7">
+        <v>44091.022900000004</v>
+      </c>
+      <c r="F165" s="7">
+        <v>55733.523300000001</v>
+      </c>
+      <c r="G165" s="7">
+        <v>35943</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166" s="4" t="s">
         <v>270</v>
       </c>
@@ -5132,8 +5720,17 @@
       <c r="D166" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E166" s="7">
+        <v>36213</v>
+      </c>
+      <c r="F166" s="7">
+        <v>46477</v>
+      </c>
+      <c r="G166" s="7">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167" s="4" t="s">
         <v>270</v>
       </c>
@@ -5146,8 +5743,17 @@
       <c r="D167" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E167" s="7">
+        <v>63322.856099999997</v>
+      </c>
+      <c r="F167" s="7">
+        <v>75211.098899999997</v>
+      </c>
+      <c r="G167" s="7">
+        <v>38290</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168" s="4" t="s">
         <v>270</v>
       </c>
@@ -5160,8 +5766,17 @@
       <c r="D168" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E168" s="7">
+        <v>52410.494100000004</v>
+      </c>
+      <c r="F168" s="7">
+        <v>66828.110400000005</v>
+      </c>
+      <c r="G168" s="7">
+        <v>24057</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169" s="4" t="s">
         <v>270</v>
       </c>
@@ -5174,8 +5789,17 @@
       <c r="D169" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E169" s="7">
+        <v>45355.138500000001</v>
+      </c>
+      <c r="F169" s="7">
+        <v>54362.9758</v>
+      </c>
+      <c r="G169" s="7">
+        <v>31968</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170" s="4" t="s">
         <v>270</v>
       </c>
@@ -5188,8 +5812,17 @@
       <c r="D170" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E170" s="7">
+        <v>62817.184000000001</v>
+      </c>
+      <c r="F170" s="7">
+        <v>74453.195000000007</v>
+      </c>
+      <c r="G170" s="7">
+        <v>45354</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171" s="4" t="s">
         <v>270</v>
       </c>
@@ -5202,8 +5835,17 @@
       <c r="D171" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E171" s="7">
+        <v>60184.671199999997</v>
+      </c>
+      <c r="F171" s="7">
+        <v>65987.709000000003</v>
+      </c>
+      <c r="G171" s="7">
+        <v>31644</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172" s="4" t="s">
         <v>270</v>
       </c>
@@ -5216,8 +5858,17 @@
       <c r="D172" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E172" s="7">
+        <v>58285.414799999999</v>
+      </c>
+      <c r="F172" s="7">
+        <v>67314.601699999999</v>
+      </c>
+      <c r="G172" s="7">
+        <v>36211</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173" s="4" t="s">
         <v>270</v>
       </c>
@@ -5230,8 +5881,17 @@
       <c r="D173" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E173" s="7">
+        <v>42945.922500000001</v>
+      </c>
+      <c r="F173" s="7">
+        <v>56201.830800000003</v>
+      </c>
+      <c r="G173" s="7">
+        <v>30237</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A174" s="4" t="s">
         <v>270</v>
       </c>
@@ -5244,8 +5904,17 @@
       <c r="D174" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E174" s="7">
+        <v>58260.1558</v>
+      </c>
+      <c r="F174" s="7">
+        <v>80353.394199999995</v>
+      </c>
+      <c r="G174" s="7">
+        <v>1584</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175" s="4" t="s">
         <v>270</v>
       </c>
@@ -5258,8 +5927,17 @@
       <c r="D175" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E175" s="7">
+        <v>46266.946600000003</v>
+      </c>
+      <c r="F175" s="7">
+        <v>56576.362200000003</v>
+      </c>
+      <c r="G175" s="7">
+        <v>49168</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176" s="4" t="s">
         <v>270</v>
       </c>
@@ -5272,8 +5950,17 @@
       <c r="D176" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E176" s="7">
+        <v>50941.976699999999</v>
+      </c>
+      <c r="F176" s="7">
+        <v>63876.736299999997</v>
+      </c>
+      <c r="G176" s="7">
+        <v>36792</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177" s="4" t="s">
         <v>270</v>
       </c>
@@ -5286,8 +5973,17 @@
       <c r="D177" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E177" s="7">
+        <v>54086.515899999999</v>
+      </c>
+      <c r="F177" s="7">
+        <v>64068.3223</v>
+      </c>
+      <c r="G177" s="7">
+        <v>19504</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178" s="4" t="s">
         <v>270</v>
       </c>
@@ -5300,8 +5996,17 @@
       <c r="D178" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E178" s="7">
+        <v>48879.826800000003</v>
+      </c>
+      <c r="F178" s="7">
+        <v>56377.423199999997</v>
+      </c>
+      <c r="G178" s="7">
+        <v>18830</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A179" s="4" t="s">
         <v>270</v>
       </c>
@@ -5314,8 +6019,17 @@
       <c r="D179" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E179" s="7">
+        <v>52409.904600000002</v>
+      </c>
+      <c r="F179" s="7">
+        <v>63083.267999999996</v>
+      </c>
+      <c r="G179" s="7">
+        <v>44151</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180" s="4" t="s">
         <v>270</v>
       </c>
@@ -5328,8 +6042,17 @@
       <c r="D180" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E180" s="7">
+        <v>65442.285100000001</v>
+      </c>
+      <c r="F180" s="7">
+        <v>77874.890400000004</v>
+      </c>
+      <c r="G180" s="7">
+        <v>36581</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181" s="4" t="s">
         <v>270</v>
       </c>
@@ -5342,8 +6065,17 @@
       <c r="D181" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E181" s="7">
+        <v>73266.001499999998</v>
+      </c>
+      <c r="F181" s="7">
+        <v>81097.512499999997</v>
+      </c>
+      <c r="G181" s="7">
+        <v>51802</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182" s="4" t="s">
         <v>270</v>
       </c>
@@ -5356,8 +6088,17 @@
       <c r="D182" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E182" s="7">
+        <v>78225.280899999998</v>
+      </c>
+      <c r="F182" s="7">
+        <v>90313.592300000004</v>
+      </c>
+      <c r="G182" s="7">
+        <v>26975</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A183" s="4" t="s">
         <v>270</v>
       </c>
@@ -5370,8 +6111,17 @@
       <c r="D183" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E183" s="7">
+        <v>75933.324299999993</v>
+      </c>
+      <c r="F183" s="7">
+        <v>98267.576000000001</v>
+      </c>
+      <c r="G183" s="7">
+        <v>35921</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184" s="4" t="s">
         <v>270</v>
       </c>
@@ -5384,8 +6134,17 @@
       <c r="D184" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E184" s="7">
+        <v>53553.965400000001</v>
+      </c>
+      <c r="F184" s="7">
+        <v>65030.7814</v>
+      </c>
+      <c r="G184" s="7">
+        <v>30203</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185" s="4" t="s">
         <v>270</v>
       </c>
@@ -5398,8 +6157,17 @@
       <c r="D185" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E185" s="7">
+        <v>54886.192300000002</v>
+      </c>
+      <c r="F185" s="7">
+        <v>64734.061699999998</v>
+      </c>
+      <c r="G185" s="7">
+        <v>10461</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186" s="4" t="s">
         <v>270</v>
       </c>
@@ -5412,8 +6180,17 @@
       <c r="D186" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E186" s="7">
+        <v>64936.966099999998</v>
+      </c>
+      <c r="F186" s="7">
+        <v>73421.685100000002</v>
+      </c>
+      <c r="G186" s="7">
+        <v>27184</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A187" s="4" t="s">
         <v>60</v>
       </c>
@@ -5426,8 +6203,17 @@
       <c r="D187" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E187" s="7">
+        <v>60184.671199999997</v>
+      </c>
+      <c r="F187" s="7">
+        <v>65987.709000000003</v>
+      </c>
+      <c r="G187" s="7">
+        <v>31644</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A188" s="4" t="s">
         <v>60</v>
       </c>
@@ -5440,8 +6226,17 @@
       <c r="D188" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E188" s="7">
+        <v>52410.494100000004</v>
+      </c>
+      <c r="F188" s="7">
+        <v>66828.110400000005</v>
+      </c>
+      <c r="G188" s="7">
+        <v>24057</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A189" s="4" t="s">
         <v>60</v>
       </c>
@@ -5454,8 +6249,17 @@
       <c r="D189" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E189" s="7">
+        <v>61316.303</v>
+      </c>
+      <c r="F189" s="7">
+        <v>69900.283800000005</v>
+      </c>
+      <c r="G189" s="7">
+        <v>26968</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A190" s="4" t="s">
         <v>60</v>
       </c>
@@ -5468,8 +6272,17 @@
       <c r="D190" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E190" s="7">
+        <v>37605.533600000002</v>
+      </c>
+      <c r="F190" s="7">
+        <v>78586.984400000001</v>
+      </c>
+      <c r="G190" s="7">
+        <v>10238</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A191" s="4" t="s">
         <v>60</v>
       </c>
@@ -5482,8 +6295,17 @@
       <c r="D191" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E191" s="7">
+        <v>64246.767800000001</v>
+      </c>
+      <c r="F191" s="7">
+        <v>77710.948699999994</v>
+      </c>
+      <c r="G191" s="7">
+        <v>20698</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A192" s="4" t="s">
         <v>60</v>
       </c>
@@ -5496,8 +6318,17 @@
       <c r="D192" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E192" s="7">
+        <v>47909.716200000003</v>
+      </c>
+      <c r="F192" s="7">
+        <v>60487.025099999999</v>
+      </c>
+      <c r="G192" s="7">
+        <v>30826</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A193" s="4" t="s">
         <v>60</v>
       </c>
@@ -5510,8 +6341,17 @@
       <c r="D193" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E193" s="7">
+        <v>104825.28449999999</v>
+      </c>
+      <c r="F193" s="7">
+        <v>128830.72169999999</v>
+      </c>
+      <c r="G193" s="7">
+        <v>36364</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A194" s="4" t="s">
         <v>60</v>
       </c>
@@ -5524,8 +6364,17 @@
       <c r="D194" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E194" s="7">
+        <v>46918.892399999997</v>
+      </c>
+      <c r="F194" s="7">
+        <v>59524.493999999999</v>
+      </c>
+      <c r="G194" s="7">
+        <v>10613</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A195" s="4" t="s">
         <v>60</v>
       </c>
@@ -5538,8 +6387,17 @@
       <c r="D195" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E195" s="7">
+        <v>44312.966099999998</v>
+      </c>
+      <c r="F195" s="7">
+        <v>53562.7356</v>
+      </c>
+      <c r="G195" s="7">
+        <v>23111</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A196" s="4" t="s">
         <v>60</v>
       </c>
@@ -5552,8 +6410,17 @@
       <c r="D196" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E196" s="7">
+        <v>93173.297000000006</v>
+      </c>
+      <c r="F196" s="7">
+        <v>111385.624</v>
+      </c>
+      <c r="G196" s="7">
+        <v>58442</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A197" s="4" t="s">
         <v>60</v>
       </c>
@@ -5566,8 +6433,17 @@
       <c r="D197" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E197" s="7">
+        <v>98841.331900000005</v>
+      </c>
+      <c r="F197" s="7">
+        <v>122243.0555</v>
+      </c>
+      <c r="G197" s="7">
+        <v>22312</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A198" s="4" t="s">
         <v>60</v>
       </c>
@@ -5580,8 +6456,17 @@
       <c r="D198" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E198" s="7">
+        <v>94297.2359</v>
+      </c>
+      <c r="F198" s="7">
+        <v>119650.6066</v>
+      </c>
+      <c r="G198" s="7">
+        <v>26141</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A199" s="4" t="s">
         <v>60</v>
       </c>
@@ -5594,8 +6479,17 @@
       <c r="D199" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E199" s="7">
+        <v>60620.723700000002</v>
+      </c>
+      <c r="F199" s="7">
+        <v>72960.822199999995</v>
+      </c>
+      <c r="G199" s="7">
+        <v>26889</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A200" s="4" t="s">
         <v>60</v>
       </c>
@@ -5608,8 +6502,17 @@
       <c r="D200" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E200" s="7">
+        <v>56657.259400000003</v>
+      </c>
+      <c r="F200" s="7">
+        <v>68952.066699999996</v>
+      </c>
+      <c r="G200" s="7">
+        <v>33769</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A201" s="4" t="s">
         <v>60</v>
       </c>
@@ -5622,8 +6525,17 @@
       <c r="D201" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E201" s="7">
+        <v>52409.904600000002</v>
+      </c>
+      <c r="F201" s="7">
+        <v>63083.267999999996</v>
+      </c>
+      <c r="G201" s="7">
+        <v>44151</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A202" s="4" t="s">
         <v>60</v>
       </c>
@@ -5636,8 +6548,17 @@
       <c r="D202" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E202" s="7">
+        <v>66530.5717</v>
+      </c>
+      <c r="F202" s="7">
+        <v>80201.871799999994</v>
+      </c>
+      <c r="G202" s="7">
+        <v>19727</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A203" s="4" t="s">
         <v>60</v>
       </c>
@@ -5650,8 +6571,17 @@
       <c r="D203" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E203" s="7">
+        <v>37833.680200000003</v>
+      </c>
+      <c r="F203" s="7">
+        <v>46816.026400000002</v>
+      </c>
+      <c r="G203" s="7">
+        <v>22851</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A204" s="4" t="s">
         <v>60</v>
       </c>
@@ -5664,8 +6594,17 @@
       <c r="D204" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E204" s="7">
+        <v>80778.946500000005</v>
+      </c>
+      <c r="F204" s="7">
+        <v>90022.046900000001</v>
+      </c>
+      <c r="G204" s="7">
+        <v>44309</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A205" s="4" t="s">
         <v>60</v>
       </c>
@@ -5678,8 +6617,17 @@
       <c r="D205" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E205" s="7">
+        <v>62962.147700000001</v>
+      </c>
+      <c r="F205" s="7">
+        <v>71251.205100000006</v>
+      </c>
+      <c r="G205" s="7">
+        <v>22246</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A206" s="4" t="s">
         <v>60</v>
       </c>
@@ -5692,8 +6640,17 @@
       <c r="D206" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E206" s="7">
+        <v>37928.792000000001</v>
+      </c>
+      <c r="F206" s="7">
+        <v>53564.7883</v>
+      </c>
+      <c r="G206" s="7">
+        <v>29750</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A207" s="4" t="s">
         <v>19</v>
       </c>
@@ -5706,8 +6663,17 @@
       <c r="D207" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E207" s="7">
+        <v>48621.962599999999</v>
+      </c>
+      <c r="F207" s="7">
+        <v>59065.2408</v>
+      </c>
+      <c r="G207" s="7">
+        <v>30072</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A208" s="4" t="s">
         <v>19</v>
       </c>
@@ -5720,8 +6686,17 @@
       <c r="D208" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E208" s="7">
+        <v>42244.986900000004</v>
+      </c>
+      <c r="F208" s="7">
+        <v>57949.0308</v>
+      </c>
+      <c r="G208" s="7">
+        <v>41740</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A209" s="4" t="s">
         <v>19</v>
       </c>
@@ -5734,8 +6709,17 @@
       <c r="D209" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E209" s="7">
+        <v>60471.663999999997</v>
+      </c>
+      <c r="F209" s="7">
+        <v>70570.445600000006</v>
+      </c>
+      <c r="G209" s="7">
+        <v>50792</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A210" s="4" t="s">
         <v>19</v>
       </c>
@@ -5748,8 +6732,17 @@
       <c r="D210" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E210" s="7">
+        <v>52410.494100000004</v>
+      </c>
+      <c r="F210" s="7">
+        <v>66828.110400000005</v>
+      </c>
+      <c r="G210" s="7">
+        <v>24057</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A211" s="4" t="s">
         <v>19</v>
       </c>
@@ -5762,8 +6755,17 @@
       <c r="D211" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E211" s="7">
+        <v>60184.671199999997</v>
+      </c>
+      <c r="F211" s="7">
+        <v>65987.709000000003</v>
+      </c>
+      <c r="G211" s="7">
+        <v>31644</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A212" s="4" t="s">
         <v>19</v>
       </c>
@@ -5776,8 +6778,17 @@
       <c r="D212" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E212" s="7">
+        <v>60471.663999999997</v>
+      </c>
+      <c r="F212" s="7">
+        <v>70570.445600000006</v>
+      </c>
+      <c r="G212" s="7">
+        <v>50792</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A213" s="4" t="s">
         <v>19</v>
       </c>
@@ -5790,8 +6801,17 @@
       <c r="D213" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E213" s="7">
+        <v>49362.042699999998</v>
+      </c>
+      <c r="F213" s="7">
+        <v>65421.099499999997</v>
+      </c>
+      <c r="G213" s="7">
+        <v>21771</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A214" s="4" t="s">
         <v>19</v>
       </c>
@@ -5804,8 +6824,17 @@
       <c r="D214" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E214" s="7">
+        <v>51434.857100000001</v>
+      </c>
+      <c r="F214" s="7">
+        <v>66967.746499999994</v>
+      </c>
+      <c r="G214" s="7">
+        <v>27763</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A215" s="4" t="s">
         <v>19</v>
       </c>
@@ -5818,8 +6847,17 @@
       <c r="D215" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E215" s="7">
+        <v>66009.695600000006</v>
+      </c>
+      <c r="F215" s="7">
+        <v>80265.121199999994</v>
+      </c>
+      <c r="G215" s="7">
+        <v>42891</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A216" s="4" t="s">
         <v>19</v>
       </c>
@@ -5832,8 +6870,17 @@
       <c r="D216" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E216" s="7">
+        <v>41273.908300000003</v>
+      </c>
+      <c r="F216" s="7">
+        <v>48310.493199999997</v>
+      </c>
+      <c r="G216" s="7">
+        <v>28254</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A217" s="4" t="s">
         <v>19</v>
       </c>
@@ -5846,8 +6893,17 @@
       <c r="D217" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E217" s="7">
+        <v>61315.587399999997</v>
+      </c>
+      <c r="F217" s="7">
+        <v>70243.738400000002</v>
+      </c>
+      <c r="G217" s="7">
+        <v>52893</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A218" s="4" t="s">
         <v>19</v>
       </c>
@@ -5860,8 +6916,17 @@
       <c r="D218" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E218" s="7">
+        <v>58304.0193</v>
+      </c>
+      <c r="F218" s="7">
+        <v>70671.428700000004</v>
+      </c>
+      <c r="G218" s="7">
+        <v>30832</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A219" s="4" t="s">
         <v>19</v>
       </c>
@@ -5874,8 +6939,17 @@
       <c r="D219" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E219" s="7">
+        <v>76045.592099999994</v>
+      </c>
+      <c r="F219" s="7">
+        <v>93289.298999999999</v>
+      </c>
+      <c r="G219" s="7">
+        <v>17089</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A220" s="4" t="s">
         <v>19</v>
       </c>
@@ -5888,8 +6962,17 @@
       <c r="D220" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E220" s="7">
+        <v>54583.4254</v>
+      </c>
+      <c r="F220" s="7">
+        <v>67917.959600000002</v>
+      </c>
+      <c r="G220" s="7">
+        <v>28896</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A221" s="4" t="s">
         <v>19</v>
       </c>
@@ -5902,8 +6985,17 @@
       <c r="D221" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E221" s="7">
+        <v>66854.906000000003</v>
+      </c>
+      <c r="F221" s="7">
+        <v>78811.983600000007</v>
+      </c>
+      <c r="G221" s="7">
+        <v>34232</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A222" s="4" t="s">
         <v>19</v>
       </c>
@@ -5916,8 +7008,17 @@
       <c r="D222" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E222" s="7">
+        <v>86042.927200000006</v>
+      </c>
+      <c r="F222" s="7">
+        <v>113432.84480000001</v>
+      </c>
+      <c r="G222" s="7">
+        <v>25381</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A223" s="4" t="s">
         <v>19</v>
       </c>
@@ -5930,8 +7031,17 @@
       <c r="D223" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E223" s="7">
+        <v>51946.512999999999</v>
+      </c>
+      <c r="F223" s="7">
+        <v>64683.800499999998</v>
+      </c>
+      <c r="G223" s="7">
+        <v>12145</v>
+      </c>
+    </row>
+    <row r="224" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A224" s="4" t="s">
         <v>19</v>
       </c>
@@ -5944,8 +7054,17 @@
       <c r="D224" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E224" s="7">
+        <v>45355.138500000001</v>
+      </c>
+      <c r="F224" s="7">
+        <v>54362.9758</v>
+      </c>
+      <c r="G224" s="7">
+        <v>31968</v>
+      </c>
+    </row>
+    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A225" s="4" t="s">
         <v>19</v>
       </c>
@@ -5958,8 +7077,17 @@
       <c r="D225" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E225" s="7">
+        <v>81588.205300000001</v>
+      </c>
+      <c r="F225" s="7">
+        <v>93422.341100000005</v>
+      </c>
+      <c r="G225" s="7">
+        <v>16651</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A226" s="4" t="s">
         <v>19</v>
       </c>
@@ -5972,8 +7100,17 @@
       <c r="D226" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E226" s="7">
+        <v>60353.151899999997</v>
+      </c>
+      <c r="F226" s="7">
+        <v>69528.578200000004</v>
+      </c>
+      <c r="G226" s="7">
+        <v>17978</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A227" s="4" t="s">
         <v>19</v>
       </c>
@@ -5986,8 +7123,17 @@
       <c r="D227" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E227" s="7">
+        <v>52629.374900000003</v>
+      </c>
+      <c r="F227" s="7">
+        <v>58028.1463</v>
+      </c>
+      <c r="G227" s="7">
+        <v>12903</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A228" s="4" t="s">
         <v>19</v>
       </c>
@@ -6000,8 +7146,17 @@
       <c r="D228" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E228" s="7">
+        <v>62759.8413</v>
+      </c>
+      <c r="F228" s="7">
+        <v>72111.412299999996</v>
+      </c>
+      <c r="G228" s="7">
+        <v>33590</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A229" s="4" t="s">
         <v>19</v>
       </c>
@@ -6014,8 +7169,17 @@
       <c r="D229" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E229" s="7">
+        <v>58633.131399999998</v>
+      </c>
+      <c r="F229" s="7">
+        <v>64986.597900000001</v>
+      </c>
+      <c r="G229" s="7">
+        <v>11948</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A230" s="4" t="s">
         <v>19</v>
       </c>
@@ -6028,8 +7192,17 @@
       <c r="D230" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E230" s="7">
+        <v>43040.570800000001</v>
+      </c>
+      <c r="F230" s="7">
+        <v>52145.329599999997</v>
+      </c>
+      <c r="G230" s="7">
+        <v>24910</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A231" s="4" t="s">
         <v>19</v>
       </c>
@@ -6042,8 +7215,17 @@
       <c r="D231" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E231" s="7">
+        <v>42945.922500000001</v>
+      </c>
+      <c r="F231" s="7">
+        <v>56201.830800000003</v>
+      </c>
+      <c r="G231" s="7">
+        <v>30237</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A232" s="4" t="s">
         <v>19</v>
       </c>
@@ -6056,8 +7238,17 @@
       <c r="D232" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E232" s="7">
+        <v>46266.946600000003</v>
+      </c>
+      <c r="F232" s="7">
+        <v>56576.362200000003</v>
+      </c>
+      <c r="G232" s="7">
+        <v>49168</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A233" s="4" t="s">
         <v>19</v>
       </c>
@@ -6070,8 +7261,17 @@
       <c r="D233" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E233" s="7">
+        <v>104825.28449999999</v>
+      </c>
+      <c r="F233" s="7">
+        <v>128830.72169999999</v>
+      </c>
+      <c r="G233" s="7">
+        <v>36364</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A234" s="4" t="s">
         <v>19</v>
       </c>
@@ -6084,8 +7284,17 @@
       <c r="D234" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E234" s="7">
+        <v>69589.362099999998</v>
+      </c>
+      <c r="F234" s="7">
+        <v>84662.419800000003</v>
+      </c>
+      <c r="G234" s="7">
+        <v>24889</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A235" s="4" t="s">
         <v>19</v>
       </c>
@@ -6098,8 +7307,17 @@
       <c r="D235" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E235" s="7">
+        <v>46918.892399999997</v>
+      </c>
+      <c r="F235" s="7">
+        <v>59524.493999999999</v>
+      </c>
+      <c r="G235" s="7">
+        <v>10613</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A236" s="4" t="s">
         <v>19</v>
       </c>
@@ -6112,8 +7330,17 @@
       <c r="D236" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E236" s="7">
+        <v>62105.866499999996</v>
+      </c>
+      <c r="F236" s="7">
+        <v>72376.570699999997</v>
+      </c>
+      <c r="G236" s="7">
+        <v>25880</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A237" s="4" t="s">
         <v>19</v>
       </c>
@@ -6126,8 +7353,17 @@
       <c r="D237" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E237" s="7">
+        <v>54726.801200000002</v>
+      </c>
+      <c r="F237" s="7">
+        <v>64162.584300000002</v>
+      </c>
+      <c r="G237" s="7">
+        <v>34258</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A238" s="4" t="s">
         <v>19</v>
       </c>
@@ -6140,8 +7376,17 @@
       <c r="D238" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E238" s="7">
+        <v>60620.723700000002</v>
+      </c>
+      <c r="F238" s="7">
+        <v>72960.822199999995</v>
+      </c>
+      <c r="G238" s="7">
+        <v>26889</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A239" s="4" t="s">
         <v>19</v>
       </c>
@@ -6154,8 +7399,17 @@
       <c r="D239" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E239" s="7">
+        <v>52409.904600000002</v>
+      </c>
+      <c r="F239" s="7">
+        <v>63083.267999999996</v>
+      </c>
+      <c r="G239" s="7">
+        <v>44151</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A240" s="4" t="s">
         <v>19</v>
       </c>
@@ -6168,8 +7422,17 @@
       <c r="D240" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E240" s="7">
+        <v>57839.249199999998</v>
+      </c>
+      <c r="F240" s="7">
+        <v>71349.785199999998</v>
+      </c>
+      <c r="G240" s="7">
+        <v>29976</v>
+      </c>
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A241" s="4" t="s">
         <v>19</v>
       </c>
@@ -6182,8 +7445,17 @@
       <c r="D241" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E241" s="7">
+        <v>52409.904600000002</v>
+      </c>
+      <c r="F241" s="7">
+        <v>63083.267999999996</v>
+      </c>
+      <c r="G241" s="7">
+        <v>44151</v>
+      </c>
+    </row>
+    <row r="242" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A242" s="4" t="s">
         <v>19</v>
       </c>
@@ -6196,8 +7468,17 @@
       <c r="D242" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E242" s="7">
+        <v>73052.0242</v>
+      </c>
+      <c r="F242" s="7">
+        <v>82554.029299999995</v>
+      </c>
+      <c r="G242" s="7">
+        <v>31911</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A243" s="4" t="s">
         <v>19</v>
       </c>
@@ -6210,8 +7491,17 @@
       <c r="D243" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E243" s="7">
+        <v>69037.25</v>
+      </c>
+      <c r="F243" s="7">
+        <v>81622.526500000007</v>
+      </c>
+      <c r="G243" s="7">
+        <v>29528</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A244" s="4" t="s">
         <v>19</v>
       </c>
@@ -6224,8 +7514,17 @@
       <c r="D244" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E244" s="7">
+        <v>46667.016199999998</v>
+      </c>
+      <c r="F244" s="7">
+        <v>53051.511899999998</v>
+      </c>
+      <c r="G244" s="7">
+        <v>39380</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A245" s="4" t="s">
         <v>19</v>
       </c>
@@ -6238,8 +7537,17 @@
       <c r="D245" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E245" s="7">
+        <v>73266.001499999998</v>
+      </c>
+      <c r="F245" s="7">
+        <v>81097.512499999997</v>
+      </c>
+      <c r="G245" s="7">
+        <v>51802</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A246" s="4" t="s">
         <v>19</v>
       </c>
@@ -6253,7 +7561,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A247" s="4" t="s">
         <v>19</v>
       </c>
@@ -6267,7 +7575,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A248" s="4" t="s">
         <v>19</v>
       </c>
@@ -6281,7 +7589,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A249" s="4" t="s">
         <v>19</v>
       </c>
@@ -6295,7 +7603,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A250" s="4" t="s">
         <v>19</v>
       </c>
@@ -6309,7 +7617,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A251" s="4" t="s">
         <v>19</v>
       </c>
@@ -6323,7 +7631,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A252" s="4" t="s">
         <v>19</v>
       </c>
@@ -6337,7 +7645,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A253" s="4" t="s">
         <v>19</v>
       </c>
@@ -6351,7 +7659,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A254" s="4" t="s">
         <v>19</v>
       </c>
@@ -6365,7 +7673,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A255" s="4" t="s">
         <v>19</v>
       </c>
@@ -6379,7 +7687,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A256" s="4" t="s">
         <v>19</v>
       </c>
@@ -6393,7 +7701,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A257" s="4" t="s">
         <v>19</v>
       </c>
@@ -6407,7 +7715,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A258" s="4" t="s">
         <v>34</v>
       </c>
@@ -6421,7 +7729,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A259" s="4" t="s">
         <v>34</v>
       </c>
@@ -6435,7 +7743,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A260" s="4" t="s">
         <v>34</v>
       </c>
@@ -6449,7 +7757,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A261" s="4" t="s">
         <v>34</v>
       </c>
@@ -6463,7 +7771,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="262" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A262" s="4" t="s">
         <v>34</v>
       </c>
@@ -6477,7 +7785,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A263" s="4" t="s">
         <v>34</v>
       </c>
@@ -6491,7 +7799,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="264" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A264" s="4" t="s">
         <v>34</v>
       </c>
@@ -6505,7 +7813,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="265" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A265" s="4" t="s">
         <v>34</v>
       </c>
@@ -6519,7 +7827,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A266" s="4" t="s">
         <v>34</v>
       </c>
@@ -6533,7 +7841,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="267" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A267" s="4" t="s">
         <v>34</v>
       </c>
@@ -6547,7 +7855,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="268" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A268" s="4" t="s">
         <v>34</v>
       </c>
@@ -6561,7 +7869,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="269" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A269" s="4" t="s">
         <v>34</v>
       </c>
@@ -6575,7 +7883,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="270" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A270" s="4" t="s">
         <v>34</v>
       </c>
@@ -6589,7 +7897,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="271" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A271" s="4" t="s">
         <v>34</v>
       </c>
@@ -6603,7 +7911,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="272" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A272" s="4" t="s">
         <v>34</v>
       </c>
@@ -6617,7 +7925,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A273" s="4" t="s">
         <v>34</v>
       </c>
@@ -6631,7 +7939,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="274" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A274" s="4" t="s">
         <v>34</v>
       </c>
@@ -6645,7 +7953,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A275" s="4" t="s">
         <v>45</v>
       </c>
@@ -6659,7 +7967,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="276" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A276" s="4" t="s">
         <v>45</v>
       </c>
@@ -6673,7 +7981,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="277" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A277" s="4" t="s">
         <v>45</v>
       </c>
@@ -6687,7 +7995,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="278" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A278" s="4" t="s">
         <v>45</v>
       </c>
@@ -6701,7 +8009,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="279" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A279" s="4" t="s">
         <v>45</v>
       </c>
@@ -6715,7 +8023,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="280" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A280" s="4" t="s">
         <v>45</v>
       </c>
@@ -6729,7 +8037,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="281" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A281" s="4" t="s">
         <v>45</v>
       </c>
@@ -6743,7 +8051,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="282" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A282" s="4" t="s">
         <v>45</v>
       </c>
@@ -6757,7 +8065,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="283" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A283" s="4" t="s">
         <v>45</v>
       </c>
@@ -6771,7 +8079,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="284" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A284" s="4" t="s">
         <v>45</v>
       </c>
@@ -6785,7 +8093,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="285" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A285" s="4" t="s">
         <v>45</v>
       </c>
@@ -6799,7 +8107,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="286" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A286" s="4" t="s">
         <v>45</v>
       </c>
@@ -6813,7 +8121,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="287" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A287" s="4" t="s">
         <v>45</v>
       </c>
@@ -6827,7 +8135,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="288" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A288" s="4" t="s">
         <v>45</v>
       </c>
@@ -6841,7 +8149,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="289" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A289" s="4" t="s">
         <v>45</v>
       </c>
@@ -6855,7 +8163,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="290" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A290" s="4" t="s">
         <v>45</v>
       </c>
@@ -6869,7 +8177,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="291" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A291" s="4" t="s">
         <v>45</v>
       </c>
@@ -6883,7 +8191,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A292" s="4" t="s">
         <v>45</v>
       </c>
@@ -6897,7 +8205,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="293" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A293" s="4" t="s">
         <v>45</v>
       </c>
@@ -6911,7 +8219,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="294" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A294" s="4" t="s">
         <v>45</v>
       </c>
@@ -6925,7 +8233,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="295" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A295" s="4" t="s">
         <v>45</v>
       </c>
@@ -6939,7 +8247,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="296" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A296" s="4" t="s">
         <v>45</v>
       </c>
@@ -6953,7 +8261,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="297" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A297" s="4" t="s">
         <v>45</v>
       </c>
@@ -6967,7 +8275,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="298" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A298" s="4" t="s">
         <v>45</v>
       </c>
@@ -6981,7 +8289,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="299" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A299" s="4" t="s">
         <v>45</v>
       </c>
@@ -6995,7 +8303,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="300" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A300" s="4" t="s">
         <v>45</v>
       </c>
@@ -7009,7 +8317,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="301" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A301" s="4" t="s">
         <v>45</v>
       </c>
@@ -7023,7 +8331,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="302" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A302" s="4" t="s">
         <v>45</v>
       </c>
@@ -7037,7 +8345,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="303" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A303" s="4" t="s">
         <v>45</v>
       </c>
@@ -7051,7 +8359,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="304" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A304" s="4" t="s">
         <v>45</v>
       </c>
@@ -7065,7 +8373,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A305" s="4" t="s">
         <v>45</v>
       </c>
@@ -7079,7 +8387,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="306" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A306" s="4" t="s">
         <v>45</v>
       </c>
@@ -7093,7 +8401,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="307" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A307" s="4" t="s">
         <v>45</v>
       </c>
@@ -7107,7 +8415,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="308" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A308" s="4" t="s">
         <v>45</v>
       </c>
@@ -7121,7 +8429,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="309" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A309" s="4" t="s">
         <v>45</v>
       </c>
@@ -7135,7 +8443,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="310" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A310" s="4" t="s">
         <v>45</v>
       </c>
@@ -7149,7 +8457,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="311" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A311" s="4" t="s">
         <v>45</v>
       </c>
@@ -7163,7 +8471,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="312" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A312" s="4" t="s">
         <v>45</v>
       </c>
@@ -7177,7 +8485,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A313" s="4" t="s">
         <v>45</v>
       </c>
@@ -7191,7 +8499,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="314" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A314" s="4" t="s">
         <v>45</v>
       </c>
@@ -7205,7 +8513,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="315" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A315" s="4" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
completed all income and population data for Navreen's added grocery stores
</commit_message>
<xml_diff>
--- a/moreWorkingData.xlsx
+++ b/moreWorkingData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mitchell.nguyen/school/senior year/spring 2019/big data/zzz letsGetThisBread/github/LetsGetThisBread/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2E942A-9ABD-1D41-B147-FD056D583C84}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FB97CE-887B-F24D-9374-6B4024125AF2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{224DDC23-A165-FE48-9542-0EB173C9A9C5}"/>
   </bookViews>
@@ -1884,8 +1884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9739F2B-2F3B-DD45-BA29-3AA82495FC82}">
   <dimension ref="A1:I315"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
-      <selection activeCell="E246" sqref="E246"/>
+    <sheetView tabSelected="1" topLeftCell="A297" workbookViewId="0">
+      <selection activeCell="C319" sqref="C319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7560,6 +7560,15 @@
       <c r="D246" t="s">
         <v>399</v>
       </c>
+      <c r="E246" s="7">
+        <v>72407.144499999995</v>
+      </c>
+      <c r="F246" s="7">
+        <v>79133.806100000002</v>
+      </c>
+      <c r="G246" s="7">
+        <v>27942</v>
+      </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A247" s="4" t="s">
@@ -7574,6 +7583,15 @@
       <c r="D247" t="s">
         <v>339</v>
       </c>
+      <c r="E247" s="7">
+        <v>37833.680200000003</v>
+      </c>
+      <c r="F247" s="7">
+        <v>46816.026400000002</v>
+      </c>
+      <c r="G247" s="7">
+        <v>22851</v>
+      </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A248" s="4" t="s">
@@ -7588,6 +7606,15 @@
       <c r="D248" t="s">
         <v>191</v>
       </c>
+      <c r="E248" s="7">
+        <v>37928.792000000001</v>
+      </c>
+      <c r="F248" s="7">
+        <v>53564.7883</v>
+      </c>
+      <c r="G248" s="7">
+        <v>29750</v>
+      </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A249" s="4" t="s">
@@ -7602,6 +7629,15 @@
       <c r="D249" t="s">
         <v>403</v>
       </c>
+      <c r="E249" s="7">
+        <v>73313.962799999994</v>
+      </c>
+      <c r="F249" s="7">
+        <v>82360.428199999995</v>
+      </c>
+      <c r="G249" s="7">
+        <v>37360</v>
+      </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A250" s="4" t="s">
@@ -7616,6 +7652,15 @@
       <c r="D250" t="s">
         <v>341</v>
       </c>
+      <c r="E250" s="7">
+        <v>80778.946500000005</v>
+      </c>
+      <c r="F250" s="7">
+        <v>90022.046900000001</v>
+      </c>
+      <c r="G250" s="7">
+        <v>44309</v>
+      </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A251" s="4" t="s">
@@ -7630,6 +7675,15 @@
       <c r="D251" t="s">
         <v>406</v>
       </c>
+      <c r="E251" s="7">
+        <v>73129.821599999996</v>
+      </c>
+      <c r="F251" s="7">
+        <v>80415.771900000007</v>
+      </c>
+      <c r="G251" s="7">
+        <v>26863</v>
+      </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A252" s="4" t="s">
@@ -7644,6 +7698,15 @@
       <c r="D252" t="s">
         <v>408</v>
       </c>
+      <c r="E252" s="7">
+        <v>68070.607000000004</v>
+      </c>
+      <c r="F252" s="7">
+        <v>73037.314799999993</v>
+      </c>
+      <c r="G252" s="7">
+        <v>45899</v>
+      </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A253" s="4" t="s">
@@ -7658,6 +7721,15 @@
       <c r="D253" t="s">
         <v>314</v>
       </c>
+      <c r="E253" s="7">
+        <v>64936.966099999998</v>
+      </c>
+      <c r="F253" s="7">
+        <v>73421.685100000002</v>
+      </c>
+      <c r="G253" s="7">
+        <v>27184</v>
+      </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A254" s="4" t="s">
@@ -7672,6 +7744,15 @@
       <c r="D254" t="s">
         <v>209</v>
       </c>
+      <c r="E254" s="7">
+        <v>65193.957900000001</v>
+      </c>
+      <c r="F254" s="7">
+        <v>75131.595100000006</v>
+      </c>
+      <c r="G254" s="7">
+        <v>40815</v>
+      </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A255" s="4" t="s">
@@ -7686,6 +7767,15 @@
       <c r="D255" t="s">
         <v>186</v>
       </c>
+      <c r="E255" s="7">
+        <v>72611.400099999999</v>
+      </c>
+      <c r="F255" s="7">
+        <v>84069.011799999993</v>
+      </c>
+      <c r="G255" s="7">
+        <v>20166</v>
+      </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A256" s="4" t="s">
@@ -7700,8 +7790,17 @@
       <c r="D256" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E256" s="7">
+        <v>58777.239800000003</v>
+      </c>
+      <c r="F256" s="7">
+        <v>67147.958599999998</v>
+      </c>
+      <c r="G256" s="7">
+        <v>36611</v>
+      </c>
+    </row>
+    <row r="257" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A257" s="4" t="s">
         <v>19</v>
       </c>
@@ -7714,8 +7813,17 @@
       <c r="D257" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E257" s="7">
+        <v>43427.327799999999</v>
+      </c>
+      <c r="F257" s="7">
+        <v>53794.748599999999</v>
+      </c>
+      <c r="G257" s="7">
+        <v>36630</v>
+      </c>
+    </row>
+    <row r="258" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A258" s="4" t="s">
         <v>34</v>
       </c>
@@ -7728,8 +7836,17 @@
       <c r="D258" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E258" s="7">
+        <v>64804.2264</v>
+      </c>
+      <c r="F258" s="7">
+        <v>79531.967600000004</v>
+      </c>
+      <c r="G258" s="7">
+        <v>21147</v>
+      </c>
+    </row>
+    <row r="259" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A259" s="4" t="s">
         <v>34</v>
       </c>
@@ -7742,8 +7859,17 @@
       <c r="D259" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E259" s="7">
+        <v>76908.244900000005</v>
+      </c>
+      <c r="F259" s="7">
+        <v>90008.385699999999</v>
+      </c>
+      <c r="G259" s="7">
+        <v>31365</v>
+      </c>
+    </row>
+    <row r="260" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A260" s="4" t="s">
         <v>34</v>
       </c>
@@ -7756,8 +7882,17 @@
       <c r="D260" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E260" s="7">
+        <v>47909.716200000003</v>
+      </c>
+      <c r="F260" s="7">
+        <v>60487.025099999999</v>
+      </c>
+      <c r="G260" s="7">
+        <v>30826</v>
+      </c>
+    </row>
+    <row r="261" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A261" s="4" t="s">
         <v>34</v>
       </c>
@@ -7770,8 +7905,17 @@
       <c r="D261" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E261" s="7">
+        <v>46918.892399999997</v>
+      </c>
+      <c r="F261" s="7">
+        <v>59524.493999999999</v>
+      </c>
+      <c r="G261" s="7">
+        <v>10613</v>
+      </c>
+    </row>
+    <row r="262" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A262" s="4" t="s">
         <v>34</v>
       </c>
@@ -7784,8 +7928,17 @@
       <c r="D262" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E262" s="7">
+        <v>93173.297000000006</v>
+      </c>
+      <c r="F262" s="7">
+        <v>111385.624</v>
+      </c>
+      <c r="G262" s="7">
+        <v>58442</v>
+      </c>
+    </row>
+    <row r="263" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A263" s="4" t="s">
         <v>34</v>
       </c>
@@ -7798,8 +7951,17 @@
       <c r="D263" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E263" s="7">
+        <v>69589.362099999998</v>
+      </c>
+      <c r="F263" s="7">
+        <v>84662.419800000003</v>
+      </c>
+      <c r="G263" s="7">
+        <v>24889</v>
+      </c>
+    </row>
+    <row r="264" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A264" s="4" t="s">
         <v>34</v>
       </c>
@@ -7812,8 +7974,17 @@
       <c r="D264" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E264" s="7">
+        <v>78392.555999999997</v>
+      </c>
+      <c r="F264" s="7">
+        <v>93426.530100000004</v>
+      </c>
+      <c r="G264" s="7">
+        <v>40407</v>
+      </c>
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A265" s="4" t="s">
         <v>34</v>
       </c>
@@ -7826,8 +7997,17 @@
       <c r="D265" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E265" s="7">
+        <v>47612.262999999999</v>
+      </c>
+      <c r="F265" s="7">
+        <v>57410.585700000003</v>
+      </c>
+      <c r="G265" s="7">
+        <v>33734</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A266" s="4" t="s">
         <v>34</v>
       </c>
@@ -7840,8 +8020,17 @@
       <c r="D266" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E266" s="7">
+        <v>51833.886500000001</v>
+      </c>
+      <c r="F266" s="7">
+        <v>64255.244200000001</v>
+      </c>
+      <c r="G266" s="7">
+        <v>33853</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A267" s="4" t="s">
         <v>34</v>
       </c>
@@ -7854,8 +8043,17 @@
       <c r="D267" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E267" s="7">
+        <v>66227.606199999995</v>
+      </c>
+      <c r="F267" s="7">
+        <v>74932.681599999996</v>
+      </c>
+      <c r="G267" s="7">
+        <v>47510</v>
+      </c>
+    </row>
+    <row r="268" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A268" s="4" t="s">
         <v>34</v>
       </c>
@@ -7868,8 +8066,17 @@
       <c r="D268" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E268" s="7">
+        <v>57182.2189</v>
+      </c>
+      <c r="F268" s="7">
+        <v>71395.290200000003</v>
+      </c>
+      <c r="G268" s="7">
+        <v>44555</v>
+      </c>
+    </row>
+    <row r="269" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A269" s="4" t="s">
         <v>34</v>
       </c>
@@ -7882,8 +8089,17 @@
       <c r="D269" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E269" s="7">
+        <v>58921.366300000002</v>
+      </c>
+      <c r="F269" s="7">
+        <v>70176.717699999994</v>
+      </c>
+      <c r="G269" s="7">
+        <v>20468</v>
+      </c>
+    </row>
+    <row r="270" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A270" s="4" t="s">
         <v>34</v>
       </c>
@@ -7896,8 +8112,17 @@
       <c r="D270" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E270" s="7">
+        <v>85126.880799999999</v>
+      </c>
+      <c r="F270" s="7">
+        <v>98424.266199999998</v>
+      </c>
+      <c r="G270" s="7">
+        <v>26722</v>
+      </c>
+    </row>
+    <row r="271" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A271" s="4" t="s">
         <v>34</v>
       </c>
@@ -7910,8 +8135,17 @@
       <c r="D271" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E271" s="7">
+        <v>40585.642800000001</v>
+      </c>
+      <c r="F271" s="7">
+        <v>49092.392599999999</v>
+      </c>
+      <c r="G271" s="7">
+        <v>31647</v>
+      </c>
+    </row>
+    <row r="272" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A272" s="4" t="s">
         <v>34</v>
       </c>
@@ -7924,8 +8158,17 @@
       <c r="D272" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E272" s="7">
+        <v>65442.285100000001</v>
+      </c>
+      <c r="F272" s="7">
+        <v>77874.890400000004</v>
+      </c>
+      <c r="G272" s="7">
+        <v>36581</v>
+      </c>
+    </row>
+    <row r="273" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A273" s="4" t="s">
         <v>34</v>
       </c>
@@ -7938,8 +8181,17 @@
       <c r="D273" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E273" s="7">
+        <v>63946.367599999998</v>
+      </c>
+      <c r="F273" s="7">
+        <v>71909.525999999998</v>
+      </c>
+      <c r="G273" s="7">
+        <v>21904</v>
+      </c>
+    </row>
+    <row r="274" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A274" s="4" t="s">
         <v>34</v>
       </c>
@@ -7952,8 +8204,17 @@
       <c r="D274" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E274" s="7">
+        <v>82732.125400000004</v>
+      </c>
+      <c r="F274" s="7">
+        <v>94032.858900000007</v>
+      </c>
+      <c r="G274" s="7">
+        <v>43673</v>
+      </c>
+    </row>
+    <row r="275" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A275" s="4" t="s">
         <v>45</v>
       </c>
@@ -7966,8 +8227,17 @@
       <c r="D275" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E275" s="7">
+        <v>64246.767800000001</v>
+      </c>
+      <c r="F275" s="7">
+        <v>77710.948699999994</v>
+      </c>
+      <c r="G275" s="7">
+        <v>20698</v>
+      </c>
+    </row>
+    <row r="276" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A276" s="4" t="s">
         <v>45</v>
       </c>
@@ -7980,8 +8250,17 @@
       <c r="D276" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E276" s="7">
+        <v>51093.423900000002</v>
+      </c>
+      <c r="F276" s="7">
+        <v>67097.652900000001</v>
+      </c>
+      <c r="G276" s="7">
+        <v>42731</v>
+      </c>
+    </row>
+    <row r="277" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A277" s="4" t="s">
         <v>45</v>
       </c>
@@ -7994,8 +8273,17 @@
       <c r="D277" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E277" s="7">
+        <v>51833.886500000001</v>
+      </c>
+      <c r="F277" s="7">
+        <v>64255.244200000001</v>
+      </c>
+      <c r="G277" s="7">
+        <v>33853</v>
+      </c>
+    </row>
+    <row r="278" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A278" s="4" t="s">
         <v>45</v>
       </c>
@@ -8008,8 +8296,17 @@
       <c r="D278" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E278" s="7">
+        <v>82556.337499999994</v>
+      </c>
+      <c r="F278" s="7">
+        <v>106971.9834</v>
+      </c>
+      <c r="G278" s="7">
+        <v>46206</v>
+      </c>
+    </row>
+    <row r="279" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A279" s="4" t="s">
         <v>45</v>
       </c>
@@ -8022,8 +8319,17 @@
       <c r="D279" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E279" s="7">
+        <v>94081.661399999997</v>
+      </c>
+      <c r="F279" s="7">
+        <v>104078.2985</v>
+      </c>
+      <c r="G279" s="7">
+        <v>31171</v>
+      </c>
+    </row>
+    <row r="280" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A280" s="4" t="s">
         <v>45</v>
       </c>
@@ -8036,8 +8342,17 @@
       <c r="D280" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E280" s="7">
+        <v>51093.423900000002</v>
+      </c>
+      <c r="F280" s="7">
+        <v>67097.652900000001</v>
+      </c>
+      <c r="G280" s="7">
+        <v>42731</v>
+      </c>
+    </row>
+    <row r="281" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A281" s="4" t="s">
         <v>45</v>
       </c>
@@ -8050,8 +8365,17 @@
       <c r="D281" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E281" s="7">
+        <v>75727.902199999997</v>
+      </c>
+      <c r="F281" s="7">
+        <v>101536.89659999999</v>
+      </c>
+      <c r="G281" s="7">
+        <v>22241</v>
+      </c>
+    </row>
+    <row r="282" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A282" s="4" t="s">
         <v>45</v>
       </c>
@@ -8064,8 +8388,17 @@
       <c r="D282" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E282" s="7">
+        <v>56657.259400000003</v>
+      </c>
+      <c r="F282" s="7">
+        <v>68952.066699999996</v>
+      </c>
+      <c r="G282" s="7">
+        <v>33769</v>
+      </c>
+    </row>
+    <row r="283" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A283" s="4" t="s">
         <v>45</v>
       </c>
@@ -8078,8 +8411,17 @@
       <c r="D283" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E283" s="7">
+        <v>71748.2745</v>
+      </c>
+      <c r="F283" s="7">
+        <v>86022.629700000005</v>
+      </c>
+      <c r="G283" s="7">
+        <v>32778</v>
+      </c>
+    </row>
+    <row r="284" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A284" s="4" t="s">
         <v>45</v>
       </c>
@@ -8092,8 +8434,17 @@
       <c r="D284" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E284" s="7">
+        <v>59070.169199999997</v>
+      </c>
+      <c r="F284" s="7">
+        <v>69812.6538</v>
+      </c>
+      <c r="G284" s="7">
+        <v>34584</v>
+      </c>
+    </row>
+    <row r="285" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A285" s="4" t="s">
         <v>45</v>
       </c>
@@ -8106,8 +8457,17 @@
       <c r="D285" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E285" s="7">
+        <v>66227.606199999995</v>
+      </c>
+      <c r="F285" s="7">
+        <v>74932.681599999996</v>
+      </c>
+      <c r="G285" s="7">
+        <v>47510</v>
+      </c>
+    </row>
+    <row r="286" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A286" s="4" t="s">
         <v>45</v>
       </c>
@@ -8120,8 +8480,17 @@
       <c r="D286" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E286" s="7">
+        <v>84572.651599999997</v>
+      </c>
+      <c r="F286" s="7">
+        <v>101222.9136</v>
+      </c>
+      <c r="G286" s="7">
+        <v>34463</v>
+      </c>
+    </row>
+    <row r="287" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A287" s="4" t="s">
         <v>45</v>
       </c>
@@ -8134,8 +8503,17 @@
       <c r="D287" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E287" s="7">
+        <v>82732.125400000004</v>
+      </c>
+      <c r="F287" s="7">
+        <v>94032.858900000007</v>
+      </c>
+      <c r="G287" s="7">
+        <v>43673</v>
+      </c>
+    </row>
+    <row r="288" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A288" s="4" t="s">
         <v>45</v>
       </c>
@@ -8148,8 +8526,17 @@
       <c r="D288" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E288" s="7">
+        <v>72812.195500000002</v>
+      </c>
+      <c r="F288" s="7">
+        <v>96772.0242</v>
+      </c>
+      <c r="G288" s="7">
+        <v>17714</v>
+      </c>
+    </row>
+    <row r="289" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A289" s="4" t="s">
         <v>45</v>
       </c>
@@ -8162,8 +8549,17 @@
       <c r="D289" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E289" s="7">
+        <v>134158.6286</v>
+      </c>
+      <c r="F289" s="7">
+        <v>157543.29089999999</v>
+      </c>
+      <c r="G289" s="7">
+        <v>25748</v>
+      </c>
+    </row>
+    <row r="290" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A290" s="4" t="s">
         <v>45</v>
       </c>
@@ -8176,8 +8572,17 @@
       <c r="D290" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E290" s="7">
+        <v>104825.28449999999</v>
+      </c>
+      <c r="F290" s="7">
+        <v>128830.72169999999</v>
+      </c>
+      <c r="G290" s="7">
+        <v>36364</v>
+      </c>
+    </row>
+    <row r="291" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A291" s="4" t="s">
         <v>45</v>
       </c>
@@ -8190,8 +8595,17 @@
       <c r="D291" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E291" s="7">
+        <v>94297.2359</v>
+      </c>
+      <c r="F291" s="7">
+        <v>119650.6066</v>
+      </c>
+      <c r="G291" s="7">
+        <v>26141</v>
+      </c>
+    </row>
+    <row r="292" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A292" s="4" t="s">
         <v>45</v>
       </c>
@@ -8204,8 +8618,17 @@
       <c r="D292" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E292" s="7">
+        <v>86310.062399999995</v>
+      </c>
+      <c r="F292" s="7">
+        <v>100545.59880000001</v>
+      </c>
+      <c r="G292" s="7">
+        <v>20419</v>
+      </c>
+    </row>
+    <row r="293" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A293" s="4" t="s">
         <v>45</v>
       </c>
@@ -8218,8 +8641,17 @@
       <c r="D293" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E293" s="7">
+        <v>120738.2426</v>
+      </c>
+      <c r="F293" s="7">
+        <v>138471.00599999999</v>
+      </c>
+      <c r="G293" s="7">
+        <v>13585</v>
+      </c>
+    </row>
+    <row r="294" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A294" s="4" t="s">
         <v>45</v>
       </c>
@@ -8232,8 +8664,17 @@
       <c r="D294" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E294" s="7">
+        <v>96608.762000000002</v>
+      </c>
+      <c r="F294" s="7">
+        <v>121401.9497</v>
+      </c>
+      <c r="G294" s="7">
+        <v>34338</v>
+      </c>
+    </row>
+    <row r="295" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A295" s="4" t="s">
         <v>45</v>
       </c>
@@ -8246,8 +8687,17 @@
       <c r="D295" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E295" s="7">
+        <v>81491.828599999993</v>
+      </c>
+      <c r="F295" s="7">
+        <v>93003.013000000006</v>
+      </c>
+      <c r="G295" s="7">
+        <v>41938</v>
+      </c>
+    </row>
+    <row r="296" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A296" s="4" t="s">
         <v>45</v>
       </c>
@@ -8260,8 +8710,17 @@
       <c r="D296" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E296" s="7">
+        <v>46918.892399999997</v>
+      </c>
+      <c r="F296" s="7">
+        <v>59524.493999999999</v>
+      </c>
+      <c r="G296" s="7">
+        <v>10613</v>
+      </c>
+    </row>
+    <row r="297" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A297" s="4" t="s">
         <v>45</v>
       </c>
@@ -8274,8 +8733,17 @@
       <c r="D297" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E297" s="7">
+        <v>84572.651599999997</v>
+      </c>
+      <c r="F297" s="7">
+        <v>101222.9136</v>
+      </c>
+      <c r="G297" s="7">
+        <v>34463</v>
+      </c>
+    </row>
+    <row r="298" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A298" s="4" t="s">
         <v>45</v>
       </c>
@@ -8288,8 +8756,17 @@
       <c r="D298" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E298" s="7">
+        <v>49287.325599999996</v>
+      </c>
+      <c r="F298" s="7">
+        <v>59856.720200000003</v>
+      </c>
+      <c r="G298" s="7">
+        <v>14115</v>
+      </c>
+    </row>
+    <row r="299" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A299" s="4" t="s">
         <v>45</v>
       </c>
@@ -8302,8 +8779,17 @@
       <c r="D299" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E299" s="7">
+        <v>42244.986900000004</v>
+      </c>
+      <c r="F299" s="7">
+        <v>57949.0308</v>
+      </c>
+      <c r="G299" s="7">
+        <v>41740</v>
+      </c>
+    </row>
+    <row r="300" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A300" s="4" t="s">
         <v>45</v>
       </c>
@@ -8316,8 +8802,17 @@
       <c r="D300" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E300" s="7">
+        <v>52410.494100000004</v>
+      </c>
+      <c r="F300" s="7">
+        <v>66828.110400000005</v>
+      </c>
+      <c r="G300" s="7">
+        <v>24057</v>
+      </c>
+    </row>
+    <row r="301" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A301" s="4" t="s">
         <v>45</v>
       </c>
@@ -8330,8 +8825,17 @@
       <c r="D301" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E301" s="7">
+        <v>42244.986900000004</v>
+      </c>
+      <c r="F301" s="7">
+        <v>57949.0308</v>
+      </c>
+      <c r="G301" s="7">
+        <v>41740</v>
+      </c>
+    </row>
+    <row r="302" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A302" s="4" t="s">
         <v>45</v>
       </c>
@@ -8344,8 +8848,17 @@
       <c r="D302" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E302" s="7">
+        <v>51434.857100000001</v>
+      </c>
+      <c r="F302" s="7">
+        <v>66967.746499999994</v>
+      </c>
+      <c r="G302" s="7">
+        <v>27763</v>
+      </c>
+    </row>
+    <row r="303" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A303" s="4" t="s">
         <v>45</v>
       </c>
@@ -8358,8 +8871,17 @@
       <c r="D303" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E303" s="7">
+        <v>63322.856099999997</v>
+      </c>
+      <c r="F303" s="7">
+        <v>75211.098899999997</v>
+      </c>
+      <c r="G303" s="7">
+        <v>38290</v>
+      </c>
+    </row>
+    <row r="304" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A304" s="4" t="s">
         <v>45</v>
       </c>
@@ -8372,8 +8894,17 @@
       <c r="D304" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E304" s="7">
+        <v>58285.414799999999</v>
+      </c>
+      <c r="F304" s="7">
+        <v>67314.601699999999</v>
+      </c>
+      <c r="G304" s="7">
+        <v>36211</v>
+      </c>
+    </row>
+    <row r="305" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A305" s="4" t="s">
         <v>45</v>
       </c>
@@ -8386,8 +8917,17 @@
       <c r="D305" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E305" s="7">
+        <v>71418.410799999998</v>
+      </c>
+      <c r="F305" s="7">
+        <v>83552.414600000004</v>
+      </c>
+      <c r="G305" s="7">
+        <v>56025</v>
+      </c>
+    </row>
+    <row r="306" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A306" s="4" t="s">
         <v>45</v>
       </c>
@@ -8400,8 +8940,17 @@
       <c r="D306" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E306" s="7">
+        <v>64848.79</v>
+      </c>
+      <c r="F306" s="7">
+        <v>80240.679799999998</v>
+      </c>
+      <c r="G306" s="7">
+        <v>26168</v>
+      </c>
+    </row>
+    <row r="307" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A307" s="4" t="s">
         <v>45</v>
       </c>
@@ -8414,8 +8963,17 @@
       <c r="D307" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E307" s="7">
+        <v>52419.156300000002</v>
+      </c>
+      <c r="F307" s="7">
+        <v>64182.508800000003</v>
+      </c>
+      <c r="G307" s="7">
+        <v>21253</v>
+      </c>
+    </row>
+    <row r="308" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A308" s="4" t="s">
         <v>45</v>
       </c>
@@ -8428,8 +8986,17 @@
       <c r="D308" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E308" s="7">
+        <v>48574.2045</v>
+      </c>
+      <c r="F308" s="7">
+        <v>56529.232600000003</v>
+      </c>
+      <c r="G308" s="7">
+        <v>35086</v>
+      </c>
+    </row>
+    <row r="309" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A309" s="4" t="s">
         <v>45</v>
       </c>
@@ -8442,8 +9009,17 @@
       <c r="D309" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E309" s="7">
+        <v>98881.172399999996</v>
+      </c>
+      <c r="F309" s="7">
+        <v>139661.7138</v>
+      </c>
+      <c r="G309" s="7">
+        <v>18340</v>
+      </c>
+    </row>
+    <row r="310" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A310" s="4" t="s">
         <v>45</v>
       </c>
@@ -8456,8 +9032,17 @@
       <c r="D310" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E310" s="7">
+        <v>81588.205300000001</v>
+      </c>
+      <c r="F310" s="7">
+        <v>93422.341100000005</v>
+      </c>
+      <c r="G310" s="7">
+        <v>16651</v>
+      </c>
+    </row>
+    <row r="311" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A311" s="4" t="s">
         <v>45</v>
       </c>
@@ -8470,8 +9055,17 @@
       <c r="D311" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E311" s="7">
+        <v>71692.024600000004</v>
+      </c>
+      <c r="F311" s="7">
+        <v>96371.055800000002</v>
+      </c>
+      <c r="G311" s="7">
+        <v>23586</v>
+      </c>
+    </row>
+    <row r="312" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A312" s="4" t="s">
         <v>45</v>
       </c>
@@ -8484,8 +9078,17 @@
       <c r="D312" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E312" s="7">
+        <v>54775.868799999997</v>
+      </c>
+      <c r="F312" s="7">
+        <v>61903.550799999997</v>
+      </c>
+      <c r="G312" s="7">
+        <v>12165</v>
+      </c>
+    </row>
+    <row r="313" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A313" s="4" t="s">
         <v>45</v>
       </c>
@@ -8498,8 +9101,17 @@
       <c r="D313" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E313" s="7">
+        <v>62817.184000000001</v>
+      </c>
+      <c r="F313" s="7">
+        <v>74453.195000000007</v>
+      </c>
+      <c r="G313" s="7">
+        <v>45354</v>
+      </c>
+    </row>
+    <row r="314" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A314" s="4" t="s">
         <v>45</v>
       </c>
@@ -8512,8 +9124,17 @@
       <c r="D314" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E314" s="7">
+        <v>54583.4254</v>
+      </c>
+      <c r="F314" s="7">
+        <v>67917.959600000002</v>
+      </c>
+      <c r="G314" s="7">
+        <v>28896</v>
+      </c>
+    </row>
+    <row r="315" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A315" s="4" t="s">
         <v>45</v>
       </c>
@@ -8525,6 +9146,15 @@
       </c>
       <c r="D315" t="s">
         <v>491</v>
+      </c>
+      <c r="E315" s="7">
+        <v>82010.159100000004</v>
+      </c>
+      <c r="F315" s="7">
+        <v>94463.125499999995</v>
+      </c>
+      <c r="G315" s="7">
+        <v>10006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>